<commit_message>
Document Modify 20181028 21:42
</commit_message>
<xml_diff>
--- a/src/main/resources/DOC/FreeProject-Develop.xlsx
+++ b/src/main/resources/DOC/FreeProject-Develop.xlsx
@@ -4,19 +4,22 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="FreePj-Doc-v1" sheetId="1" r:id="rId1"/>
     <sheet name="FreePj-Develop-Ready" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Developer-Read" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'FreePj-Doc-v1'!$C$18:$D$18</definedName>
+  </definedNames>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="61">
   <si>
     <t>2.功能设想:</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -133,12 +136,162 @@
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>Mysql驱动升级</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>POM文件：</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;!-- MySQL 依赖 --&gt;</t>
+  </si>
+  <si>
+    <t>&lt;dependency&gt;</t>
+  </si>
+  <si>
+    <t>&lt;groupId&gt;mysql&lt;/groupId&gt;</t>
+  </si>
+  <si>
+    <t>&lt;artifactId&gt;mysql-connector-java&lt;/artifactId&gt;</t>
+  </si>
+  <si>
+    <t>&lt;version&gt;8.0.11&lt;/version&gt;</t>
+  </si>
+  <si>
+    <t>&lt;/dependency&gt;</t>
+  </si>
+  <si>
+    <t>旧版本</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>新版本</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;version&gt;5.1.42&lt;/version&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>jdbc.properties</t>
+  </si>
+  <si>
+    <t>#driver=com.mysql.jdbc.Driver</t>
+  </si>
+  <si>
+    <t>#url=jdbc:mysql://localhost:3306/freePj</t>
+  </si>
+  <si>
+    <t>driver=com.mysql.cj.jdbc.Driver</t>
+  </si>
+  <si>
+    <t>url=jdbc:mysql://localhost:3306/freePj?characterEncoding=utf-8&amp;serverTimezone=UTC&amp;useSSL=false</t>
+  </si>
+  <si>
+    <t>时间控件：</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>位置</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>代码</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>function bootstrapDateChange(currentElement, obj){</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> var dates = $('input[name='+ obj +']');</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> if (dates.length &gt; 1) {</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> return false;</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> }else {</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> $(dates[0]).val(Date.parse(new Date($(currentElement).val()))); </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> return true;</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> }</t>
+  </si>
+  <si>
+    <t>main.jsp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;!-- Date format of Search Condition Area [Start]--&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div class="col-lg-3 col-md-1 col-sm-2 col-xs-4" style="padding: 5px 0px 0px 10px;"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;label for="name" class="font-16"&gt;注册时间&lt;/label&gt;</t>
+  </si>
+  <si>
+    <t>&lt;span class="label label-default"&gt;(Register Time)&lt;/span&gt;</t>
+  </si>
+  <si>
+    <t>&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div class="col-lg-4 col-md-3 col-sm-4 col-xs-7"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;input placeholder="点击输入注册时间" id=""registerTime""</t>
+  </si>
+  <si>
+    <t>class="form-control bootstrap-date" type="text" onchange="bootstrapDateChange(this,'registerTime')"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;input name="registerTime" type="hidden"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;!-- Date format of Search Condition Area [End]--&gt;</t>
+  </si>
+  <si>
+    <t>sys0501.jsp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.角色代码:</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>角色</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>管理员</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>开发者</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>体验者</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -196,8 +349,32 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="8" tint="-0.249977111117893"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -210,8 +387,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -219,11 +402,106 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -236,6 +514,8 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -250,7 +530,34 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -710,6 +1017,200 @@
             <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
             <a:t>文件夹下</a:t>
           </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="矩形标注 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6534150" y="3800475"/>
+          <a:ext cx="2286000" cy="942975"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -68333"/>
+            <a:gd name="adj2" fmla="val -71528"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1600"/>
+            <a:t>设置隐藏域</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1600"/>
+            <a:t>,name</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1600"/>
+            <a:t>和</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1600"/>
+            <a:t>bean</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1600"/>
+            <a:t>中的</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1600"/>
+            <a:t>searchDto</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1600"/>
+            <a:t>名字一致</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="矩形标注 2"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10420350" y="1866900"/>
+          <a:ext cx="1933575" cy="942975"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -55808"/>
+            <a:gd name="adj2" fmla="val 88763"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
+            <a:t>使用时间控件时</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
+            <a:t>,</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
+            <a:t>将</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
+            <a:t>searchDto</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
+            <a:t>的</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
+            <a:t>name</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
+            <a:t>也放入</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
+            <a:t>onchang</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
+            <a:t>事件</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
+            <a:t>(</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
+            <a:t>为了给隐藏域赋值</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
+            <a:t>)</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -1008,10 +1509,10 @@
   <sheetPr>
     <tabColor rgb="FF002060"/>
   </sheetPr>
-  <dimension ref="A1:P15"/>
+  <dimension ref="A1:P21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1023,20 +1524,20 @@
       <c r="A1" s="3"/>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
       <c r="J1" s="3"/>
       <c r="K1" s="3"/>
       <c r="L1" s="3"/>
       <c r="M1" s="3"/>
       <c r="N1" s="3"/>
-      <c r="O1" s="8" t="s">
+      <c r="O1" s="10" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1046,81 +1547,81 @@
       <c r="C2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
       <c r="J2" s="3"/>
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
       <c r="N2" s="3"/>
-      <c r="O2" s="8"/>
+      <c r="O2" s="10"/>
       <c r="P2" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12"/>
-      <c r="J3" s="12"/>
-      <c r="K3" s="12"/>
-      <c r="L3" s="12"/>
-      <c r="M3" s="12"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="14"/>
+      <c r="L3" s="14"/>
+      <c r="M3" s="14"/>
       <c r="O3" s="2"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="B4" s="12"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="12"/>
-      <c r="K4" s="12"/>
-      <c r="L4" s="12"/>
-      <c r="M4" s="12"/>
+      <c r="B4" s="14"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="14"/>
+      <c r="L4" s="14"/>
+      <c r="M4" s="14"/>
       <c r="O4" s="6">
         <v>101</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="11"/>
+      <c r="C5" s="13"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.15">
       <c r="C8" s="5">
@@ -1155,32 +1656,70 @@
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="D14" s="10" t="s">
+      <c r="D14" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10"/>
-      <c r="I14" s="10"/>
-      <c r="J14" s="10"/>
-      <c r="K14" s="10"/>
-      <c r="L14" s="10"/>
-      <c r="M14" s="10"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="12"/>
+      <c r="J14" s="12"/>
+      <c r="K14" s="12"/>
+      <c r="L14" s="12"/>
+      <c r="M14" s="12"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="10"/>
-      <c r="I15" s="10"/>
-      <c r="J15" s="10"/>
-      <c r="K15" s="10"/>
-      <c r="L15" s="10"/>
-      <c r="M15" s="10"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="12"/>
+      <c r="I15" s="12"/>
+      <c r="J15" s="12"/>
+      <c r="K15" s="12"/>
+      <c r="L15" s="12"/>
+      <c r="M15" s="12"/>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="B17" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="C18" s="32" t="s">
+        <v>57</v>
+      </c>
+      <c r="D18" s="32" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="C19" s="33" t="s">
+        <v>58</v>
+      </c>
+      <c r="D19" s="33">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="C20" s="33" t="s">
+        <v>59</v>
+      </c>
+      <c r="D20" s="33">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="C21" s="33" t="s">
+        <v>60</v>
+      </c>
+      <c r="D21" s="33">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
+  <autoFilter ref="C18:D18"/>
   <mergeCells count="7">
     <mergeCell ref="O1:O2"/>
     <mergeCell ref="D1:I2"/>
@@ -1201,32 +1740,211 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:N100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O9" sqref="O9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H97" sqref="H97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="14"/>
+      <c r="C6" s="9"/>
+    </row>
+    <row r="82" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A82" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="B82" s="17"/>
+    </row>
+    <row r="83" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="B83" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C83" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="D83" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E83" s="8"/>
+      <c r="F83" s="8"/>
+      <c r="G83" s="8"/>
+      <c r="H83" s="8"/>
+      <c r="I83" s="8"/>
+      <c r="J83" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="K83" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="L83" s="8"/>
+      <c r="M83" s="8"/>
+      <c r="N83" s="8"/>
+    </row>
+    <row r="84" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="C84" s="18"/>
+      <c r="D84" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E84" s="8"/>
+      <c r="F84" s="8"/>
+      <c r="G84" s="8"/>
+      <c r="H84" s="8"/>
+      <c r="I84" s="8"/>
+      <c r="J84" s="18"/>
+      <c r="K84" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="L84" s="8"/>
+    </row>
+    <row r="85" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="C85" s="18"/>
+      <c r="D85" s="8"/>
+      <c r="E85" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="F85" s="8"/>
+      <c r="G85" s="8"/>
+      <c r="H85" s="8"/>
+      <c r="I85" s="8"/>
+      <c r="J85" s="18"/>
+      <c r="K85" s="8"/>
+      <c r="L85" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="86" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="C86" s="18"/>
+      <c r="D86" s="8"/>
+      <c r="E86" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F86" s="8"/>
+      <c r="G86" s="8"/>
+      <c r="H86" s="8"/>
+      <c r="I86" s="8"/>
+      <c r="J86" s="18"/>
+      <c r="K86" s="8"/>
+      <c r="L86" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="87" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="C87" s="18"/>
+      <c r="D87" s="8"/>
+      <c r="E87" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="F87" s="8"/>
+      <c r="G87" s="8"/>
+      <c r="H87" s="8"/>
+      <c r="I87" s="8"/>
+      <c r="J87" s="18"/>
+      <c r="K87" s="8"/>
+      <c r="L87" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="88" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="C88" s="18"/>
+      <c r="D88" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E88" s="8"/>
+      <c r="F88" s="8"/>
+      <c r="G88" s="8"/>
+      <c r="H88" s="8"/>
+      <c r="I88" s="8"/>
+      <c r="J88" s="18"/>
+      <c r="K88" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="L88" s="8"/>
+    </row>
+    <row r="89" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="C89" s="18"/>
+      <c r="D89" s="8"/>
+      <c r="J89" s="18"/>
+    </row>
+    <row r="90" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="C90" s="18"/>
+      <c r="J90" s="18"/>
+    </row>
+    <row r="91" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="C91" s="18"/>
+      <c r="J91" s="18"/>
+    </row>
+    <row r="92" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="C92" s="18"/>
+      <c r="J92" s="18"/>
+    </row>
+    <row r="93" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A93" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="B93" s="16"/>
+      <c r="C93" s="18"/>
+      <c r="D93" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="J93" s="18"/>
+      <c r="K93" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="94" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="C94" s="18"/>
+      <c r="D94" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="J94" s="18"/>
+      <c r="K94" s="8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="95" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="C95" s="18"/>
+      <c r="J95" s="18"/>
+    </row>
+    <row r="96" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="C96" s="18"/>
+      <c r="J96" s="18"/>
+    </row>
+    <row r="97" spans="3:10" x14ac:dyDescent="0.15">
+      <c r="C97" s="18"/>
+      <c r="J97" s="18"/>
+    </row>
+    <row r="98" spans="3:10" x14ac:dyDescent="0.15">
+      <c r="C98" s="18"/>
+      <c r="J98" s="18"/>
+    </row>
+    <row r="99" spans="3:10" x14ac:dyDescent="0.15">
+      <c r="C99" s="18"/>
+      <c r="J99" s="18"/>
+    </row>
+    <row r="100" spans="3:10" x14ac:dyDescent="0.15">
+      <c r="J100" s="18"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="5">
     <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A82:B82"/>
+    <mergeCell ref="C83:C99"/>
+    <mergeCell ref="J83:J100"/>
+    <mergeCell ref="A93:B93"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1237,13 +1955,640 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:S28"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="B1" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="A2" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="22"/>
+      <c r="K2" s="22"/>
+      <c r="L2" s="22"/>
+      <c r="M2" s="22"/>
+      <c r="N2" s="22"/>
+      <c r="O2" s="22"/>
+      <c r="P2" s="22"/>
+      <c r="Q2" s="22"/>
+      <c r="R2" s="22"/>
+      <c r="S2" s="23"/>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="A3" s="24"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25" t="s">
+        <v>36</v>
+      </c>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
+      <c r="K3" s="25"/>
+      <c r="L3" s="25"/>
+      <c r="M3" s="25"/>
+      <c r="N3" s="25"/>
+      <c r="O3" s="25"/>
+      <c r="P3" s="25"/>
+      <c r="Q3" s="25"/>
+      <c r="R3" s="25"/>
+      <c r="S3" s="26"/>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="A4" s="24"/>
+      <c r="B4" s="25"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4" s="25"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="25"/>
+      <c r="H4" s="25"/>
+      <c r="I4" s="25"/>
+      <c r="J4" s="25"/>
+      <c r="K4" s="25"/>
+      <c r="L4" s="25"/>
+      <c r="M4" s="25"/>
+      <c r="N4" s="25"/>
+      <c r="O4" s="25"/>
+      <c r="P4" s="25"/>
+      <c r="Q4" s="25"/>
+      <c r="R4" s="25"/>
+      <c r="S4" s="26"/>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="A5" s="24"/>
+      <c r="B5" s="25"/>
+      <c r="C5" s="25"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="F5" s="25"/>
+      <c r="G5" s="25"/>
+      <c r="H5" s="25"/>
+      <c r="I5" s="25"/>
+      <c r="J5" s="25"/>
+      <c r="K5" s="25"/>
+      <c r="L5" s="25"/>
+      <c r="M5" s="25"/>
+      <c r="N5" s="25"/>
+      <c r="O5" s="25"/>
+      <c r="P5" s="25"/>
+      <c r="Q5" s="25"/>
+      <c r="R5" s="25"/>
+      <c r="S5" s="26"/>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="A6" s="24"/>
+      <c r="B6" s="25"/>
+      <c r="C6" s="25"/>
+      <c r="D6" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="E6" s="25"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="25"/>
+      <c r="H6" s="25"/>
+      <c r="I6" s="25"/>
+      <c r="J6" s="25"/>
+      <c r="K6" s="25"/>
+      <c r="L6" s="25"/>
+      <c r="M6" s="25"/>
+      <c r="N6" s="25"/>
+      <c r="O6" s="25"/>
+      <c r="P6" s="25"/>
+      <c r="Q6" s="25"/>
+      <c r="R6" s="25"/>
+      <c r="S6" s="26"/>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="A7" s="24"/>
+      <c r="B7" s="25"/>
+      <c r="C7" s="25"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="F7" s="25"/>
+      <c r="G7" s="25"/>
+      <c r="H7" s="25"/>
+      <c r="I7" s="25"/>
+      <c r="J7" s="25"/>
+      <c r="K7" s="25"/>
+      <c r="L7" s="25"/>
+      <c r="M7" s="25"/>
+      <c r="N7" s="25"/>
+      <c r="O7" s="25"/>
+      <c r="P7" s="25"/>
+      <c r="Q7" s="25"/>
+      <c r="R7" s="25"/>
+      <c r="S7" s="26"/>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="A8" s="24"/>
+      <c r="B8" s="25"/>
+      <c r="C8" s="25"/>
+      <c r="D8" s="25"/>
+      <c r="E8" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="F8" s="25"/>
+      <c r="G8" s="25"/>
+      <c r="H8" s="25"/>
+      <c r="I8" s="25"/>
+      <c r="J8" s="25"/>
+      <c r="K8" s="25"/>
+      <c r="L8" s="25"/>
+      <c r="M8" s="25"/>
+      <c r="N8" s="25"/>
+      <c r="O8" s="25"/>
+      <c r="P8" s="25"/>
+      <c r="Q8" s="25"/>
+      <c r="R8" s="25"/>
+      <c r="S8" s="26"/>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="A9" s="24"/>
+      <c r="B9" s="25"/>
+      <c r="C9" s="25"/>
+      <c r="D9" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="E9" s="25"/>
+      <c r="F9" s="25"/>
+      <c r="G9" s="25"/>
+      <c r="H9" s="25"/>
+      <c r="I9" s="25"/>
+      <c r="J9" s="25"/>
+      <c r="K9" s="25"/>
+      <c r="L9" s="25"/>
+      <c r="M9" s="25"/>
+      <c r="N9" s="25"/>
+      <c r="O9" s="25"/>
+      <c r="P9" s="25"/>
+      <c r="Q9" s="25"/>
+      <c r="R9" s="25"/>
+      <c r="S9" s="26"/>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="A10" s="24"/>
+      <c r="B10" s="25"/>
+      <c r="C10" s="25"/>
+      <c r="D10" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="E10" s="25"/>
+      <c r="F10" s="25"/>
+      <c r="G10" s="25"/>
+      <c r="H10" s="25"/>
+      <c r="I10" s="25"/>
+      <c r="J10" s="25"/>
+      <c r="K10" s="25"/>
+      <c r="L10" s="25"/>
+      <c r="M10" s="25"/>
+      <c r="N10" s="25"/>
+      <c r="O10" s="25"/>
+      <c r="P10" s="25"/>
+      <c r="Q10" s="25"/>
+      <c r="R10" s="25"/>
+      <c r="S10" s="26"/>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="A11" s="24"/>
+      <c r="B11" s="25"/>
+      <c r="C11" s="25"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25"/>
+      <c r="G11" s="25"/>
+      <c r="H11" s="25"/>
+      <c r="I11" s="25"/>
+      <c r="J11" s="25"/>
+      <c r="K11" s="25"/>
+      <c r="L11" s="25"/>
+      <c r="M11" s="25"/>
+      <c r="N11" s="25"/>
+      <c r="O11" s="25"/>
+      <c r="P11" s="25"/>
+      <c r="Q11" s="25"/>
+      <c r="R11" s="25"/>
+      <c r="S11" s="26"/>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="A12" s="24"/>
+      <c r="B12" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="C12" s="25"/>
+      <c r="D12" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="E12" s="25"/>
+      <c r="F12" s="25"/>
+      <c r="G12" s="25"/>
+      <c r="H12" s="25"/>
+      <c r="I12" s="25"/>
+      <c r="J12" s="25"/>
+      <c r="K12" s="25"/>
+      <c r="L12" s="25"/>
+      <c r="M12" s="25"/>
+      <c r="N12" s="25"/>
+      <c r="O12" s="25"/>
+      <c r="P12" s="25"/>
+      <c r="Q12" s="25"/>
+      <c r="R12" s="25"/>
+      <c r="S12" s="26"/>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="A13" s="24"/>
+      <c r="B13" s="25"/>
+      <c r="C13" s="25"/>
+      <c r="D13" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="E13" s="25"/>
+      <c r="F13" s="25"/>
+      <c r="G13" s="25"/>
+      <c r="H13" s="25"/>
+      <c r="I13" s="25"/>
+      <c r="J13" s="25"/>
+      <c r="K13" s="25"/>
+      <c r="L13" s="25"/>
+      <c r="M13" s="25"/>
+      <c r="N13" s="25"/>
+      <c r="O13" s="25"/>
+      <c r="P13" s="25"/>
+      <c r="Q13" s="25"/>
+      <c r="R13" s="25"/>
+      <c r="S13" s="26"/>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="A14" s="24"/>
+      <c r="B14" s="25"/>
+      <c r="C14" s="25"/>
+      <c r="D14" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="E14" s="25"/>
+      <c r="F14" s="25"/>
+      <c r="G14" s="25"/>
+      <c r="H14" s="25"/>
+      <c r="I14" s="25"/>
+      <c r="J14" s="25"/>
+      <c r="K14" s="25"/>
+      <c r="L14" s="25"/>
+      <c r="M14" s="25"/>
+      <c r="N14" s="25"/>
+      <c r="O14" s="25"/>
+      <c r="P14" s="25"/>
+      <c r="Q14" s="25"/>
+      <c r="R14" s="25"/>
+      <c r="S14" s="26"/>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="A15" s="24"/>
+      <c r="B15" s="25"/>
+      <c r="C15" s="25"/>
+      <c r="D15" s="25"/>
+      <c r="E15" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="F15" s="25"/>
+      <c r="G15" s="25"/>
+      <c r="H15" s="25"/>
+      <c r="I15" s="25"/>
+      <c r="J15" s="25"/>
+      <c r="K15" s="25"/>
+      <c r="L15" s="25"/>
+      <c r="M15" s="25"/>
+      <c r="N15" s="25"/>
+      <c r="O15" s="25"/>
+      <c r="P15" s="25"/>
+      <c r="Q15" s="25"/>
+      <c r="R15" s="25"/>
+      <c r="S15" s="26"/>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="A16" s="24"/>
+      <c r="B16" s="25"/>
+      <c r="C16" s="25"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="F16" s="25"/>
+      <c r="G16" s="25"/>
+      <c r="H16" s="25"/>
+      <c r="I16" s="25"/>
+      <c r="J16" s="25"/>
+      <c r="K16" s="25"/>
+      <c r="L16" s="25"/>
+      <c r="M16" s="25"/>
+      <c r="N16" s="25"/>
+      <c r="O16" s="25"/>
+      <c r="P16" s="25"/>
+      <c r="Q16" s="25"/>
+      <c r="R16" s="25"/>
+      <c r="S16" s="26"/>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="A17" s="24"/>
+      <c r="B17" s="25"/>
+      <c r="C17" s="25"/>
+      <c r="D17" s="25" t="s">
+        <v>49</v>
+      </c>
+      <c r="E17" s="25"/>
+      <c r="F17" s="25"/>
+      <c r="G17" s="25"/>
+      <c r="H17" s="25"/>
+      <c r="I17" s="25"/>
+      <c r="J17" s="25"/>
+      <c r="K17" s="25"/>
+      <c r="L17" s="25"/>
+      <c r="M17" s="25"/>
+      <c r="N17" s="25"/>
+      <c r="O17" s="25"/>
+      <c r="P17" s="25"/>
+      <c r="Q17" s="25"/>
+      <c r="R17" s="25"/>
+      <c r="S17" s="26"/>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="A18" s="24"/>
+      <c r="B18" s="25"/>
+      <c r="C18" s="25"/>
+      <c r="D18" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="E18" s="25"/>
+      <c r="F18" s="25"/>
+      <c r="G18" s="25"/>
+      <c r="H18" s="25"/>
+      <c r="I18" s="25"/>
+      <c r="J18" s="25"/>
+      <c r="K18" s="25"/>
+      <c r="L18" s="25"/>
+      <c r="M18" s="25"/>
+      <c r="N18" s="25"/>
+      <c r="O18" s="25"/>
+      <c r="P18" s="25"/>
+      <c r="Q18" s="25"/>
+      <c r="R18" s="25"/>
+      <c r="S18" s="26"/>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="A19" s="24"/>
+      <c r="B19" s="25"/>
+      <c r="C19" s="25"/>
+      <c r="D19" s="25"/>
+      <c r="E19" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="F19" s="25"/>
+      <c r="G19" s="25"/>
+      <c r="H19" s="25"/>
+      <c r="I19" s="25"/>
+      <c r="J19" s="25"/>
+      <c r="K19" s="25"/>
+      <c r="L19" s="25"/>
+      <c r="M19" s="25"/>
+      <c r="N19" s="25"/>
+      <c r="O19" s="25"/>
+      <c r="P19" s="25"/>
+      <c r="Q19" s="25"/>
+      <c r="R19" s="25"/>
+      <c r="S19" s="26"/>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="A20" s="24"/>
+      <c r="B20" s="25"/>
+      <c r="C20" s="25"/>
+      <c r="D20" s="25"/>
+      <c r="E20" s="25"/>
+      <c r="F20" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="G20" s="25"/>
+      <c r="H20" s="25"/>
+      <c r="I20" s="25"/>
+      <c r="J20" s="25"/>
+      <c r="K20" s="25"/>
+      <c r="L20" s="30"/>
+      <c r="M20" s="30"/>
+      <c r="N20" s="30"/>
+      <c r="O20" s="30"/>
+      <c r="P20" s="30"/>
+      <c r="Q20" s="25"/>
+      <c r="R20" s="25"/>
+      <c r="S20" s="26"/>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="A21" s="24"/>
+      <c r="B21" s="25"/>
+      <c r="C21" s="25"/>
+      <c r="D21" s="25"/>
+      <c r="E21" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="F21" s="31"/>
+      <c r="G21" s="31"/>
+      <c r="H21" s="31"/>
+      <c r="I21" s="31"/>
+      <c r="J21" s="25"/>
+      <c r="K21" s="25"/>
+      <c r="L21" s="25"/>
+      <c r="M21" s="25"/>
+      <c r="N21" s="25"/>
+      <c r="O21" s="25"/>
+      <c r="P21" s="25"/>
+      <c r="Q21" s="25"/>
+      <c r="R21" s="25"/>
+      <c r="S21" s="26"/>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="A22" s="24"/>
+      <c r="B22" s="25"/>
+      <c r="C22" s="25"/>
+      <c r="D22" s="25" t="s">
+        <v>49</v>
+      </c>
+      <c r="E22" s="25"/>
+      <c r="F22" s="25"/>
+      <c r="G22" s="25"/>
+      <c r="H22" s="25"/>
+      <c r="I22" s="25"/>
+      <c r="J22" s="25"/>
+      <c r="K22" s="25"/>
+      <c r="L22" s="25"/>
+      <c r="M22" s="25"/>
+      <c r="N22" s="25"/>
+      <c r="O22" s="25"/>
+      <c r="P22" s="25"/>
+      <c r="Q22" s="25"/>
+      <c r="R22" s="25"/>
+      <c r="S22" s="26"/>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="A23" s="24"/>
+      <c r="B23" s="25"/>
+      <c r="C23" s="25"/>
+      <c r="D23" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="E23" s="25"/>
+      <c r="F23" s="25"/>
+      <c r="G23" s="25"/>
+      <c r="H23" s="25"/>
+      <c r="I23" s="25"/>
+      <c r="J23" s="25"/>
+      <c r="K23" s="25"/>
+      <c r="L23" s="25"/>
+      <c r="M23" s="25"/>
+      <c r="N23" s="25"/>
+      <c r="O23" s="25"/>
+      <c r="P23" s="25"/>
+      <c r="Q23" s="25"/>
+      <c r="R23" s="25"/>
+      <c r="S23" s="26"/>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="A24" s="24"/>
+      <c r="B24" s="25"/>
+      <c r="C24" s="25"/>
+      <c r="D24" s="25"/>
+      <c r="E24" s="25"/>
+      <c r="F24" s="25"/>
+      <c r="G24" s="25"/>
+      <c r="H24" s="25"/>
+      <c r="I24" s="25"/>
+      <c r="J24" s="25"/>
+      <c r="K24" s="25"/>
+      <c r="L24" s="25"/>
+      <c r="M24" s="25"/>
+      <c r="N24" s="25"/>
+      <c r="O24" s="25"/>
+      <c r="P24" s="25"/>
+      <c r="Q24" s="25"/>
+      <c r="R24" s="25"/>
+      <c r="S24" s="26"/>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="A25" s="24"/>
+      <c r="B25" s="25"/>
+      <c r="C25" s="25"/>
+      <c r="D25" s="25"/>
+      <c r="E25" s="25"/>
+      <c r="F25" s="25"/>
+      <c r="G25" s="25"/>
+      <c r="H25" s="25"/>
+      <c r="I25" s="25"/>
+      <c r="J25" s="25"/>
+      <c r="K25" s="25"/>
+      <c r="L25" s="25"/>
+      <c r="M25" s="25"/>
+      <c r="N25" s="25"/>
+      <c r="O25" s="25"/>
+      <c r="P25" s="25"/>
+      <c r="Q25" s="25"/>
+      <c r="R25" s="25"/>
+      <c r="S25" s="26"/>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="A26" s="24"/>
+      <c r="B26" s="25"/>
+      <c r="C26" s="25"/>
+      <c r="D26" s="25"/>
+      <c r="E26" s="25"/>
+      <c r="F26" s="25"/>
+      <c r="G26" s="25"/>
+      <c r="H26" s="25"/>
+      <c r="I26" s="25"/>
+      <c r="J26" s="25"/>
+      <c r="K26" s="25"/>
+      <c r="L26" s="25"/>
+      <c r="M26" s="25"/>
+      <c r="N26" s="25"/>
+      <c r="O26" s="25"/>
+      <c r="P26" s="25"/>
+      <c r="Q26" s="25"/>
+      <c r="R26" s="25"/>
+      <c r="S26" s="26"/>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="A27" s="24"/>
+      <c r="B27" s="25"/>
+      <c r="C27" s="25"/>
+      <c r="D27" s="25"/>
+      <c r="E27" s="25"/>
+      <c r="F27" s="25"/>
+      <c r="G27" s="25"/>
+      <c r="H27" s="25"/>
+      <c r="I27" s="25"/>
+      <c r="J27" s="25"/>
+      <c r="K27" s="25"/>
+      <c r="L27" s="25"/>
+      <c r="M27" s="25"/>
+      <c r="N27" s="25"/>
+      <c r="O27" s="25"/>
+      <c r="P27" s="25"/>
+      <c r="Q27" s="25"/>
+      <c r="R27" s="25"/>
+      <c r="S27" s="26"/>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="A28" s="27"/>
+      <c r="B28" s="28"/>
+      <c r="C28" s="28"/>
+      <c r="D28" s="28"/>
+      <c r="E28" s="28"/>
+      <c r="F28" s="28"/>
+      <c r="G28" s="28"/>
+      <c r="H28" s="28"/>
+      <c r="I28" s="28"/>
+      <c r="J28" s="28"/>
+      <c r="K28" s="28"/>
+      <c r="L28" s="28"/>
+      <c r="M28" s="28"/>
+      <c r="N28" s="28"/>
+      <c r="O28" s="28"/>
+      <c r="P28" s="28"/>
+      <c r="Q28" s="28"/>
+      <c r="R28" s="28"/>
+      <c r="S28" s="29"/>
+    </row>
+  </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Document Add And DB Data Add 20181031 22:04
</commit_message>
<xml_diff>
--- a/src/main/resources/DOC/FreeProject-Develop.xlsx
+++ b/src/main/resources/DOC/FreeProject-Develop.xlsx
@@ -12,6 +12,7 @@
     <sheet name="Developer-Read" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Developer-Read'!$A$1:$B$2</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'FreePj-Doc-v1'!$C$18:$D$18</definedName>
   </definedNames>
   <calcPr calcId="122211"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="103">
   <si>
     <t>2.功能设想:</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -286,12 +287,149 @@
     <t>体验者</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>4.权限代码:</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>权限</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>检索权限</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>更新权限</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>录入权限</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>下载权限</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>管理员权限</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sys0501SearchDto.java</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>private Date registerTime;</t>
+  </si>
+  <si>
+    <t>private long registerTimeTimestamp;</t>
+  </si>
+  <si>
+    <t>loadDateComponent();</t>
+  </si>
+  <si>
+    <t>JS部分(main.jsp):</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>class="form-control bootstrap-date" type="text" onchange="bootstrapDateChange(this,'registerTime')"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> value="&lt;fmt:formatDate value="${sys0501SearchDto.registerTime }" pattern="yyyy-MM-dd HH:mm:ss"/&gt;"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;input name="registerTime" type="hidden" value="${sys0501SearchDto.registerTimeTimestamp }"&gt;</t>
+  </si>
+  <si>
+    <t>多选框控件:</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;div class="form-group"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div class="col-lg-3 col-md-1 col-sm-2 col-xs-4 "&gt;</t>
+  </si>
+  <si>
+    <t>&lt;label for="name"&gt;权&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;限</t>
+  </si>
+  <si>
+    <t>&lt;span class="label label-default"&gt;(Authority)&lt;/span&gt;</t>
+  </si>
+  <si>
+    <t>&lt;/label&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div class="col-lg-4 col-md-4 col-sm-5 col-xs-10"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;select class="form-control" multiple="multiple" name="authorityId"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;c:forEach items="${authorityList }" var="authority"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;c:set var="printAuthorityFlag" value="1"/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;c:choose&gt;</t>
+  </si>
+  <si>
+    <t>&lt;c:when test="${sys0501SearchDto.authorityId != null}"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;c:forEach items="${sys0501SearchDto.authorityId }" var="authorityBySearch" varStatus="authorityBySearchIndex"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;c:when test="${authority.authorityId == authorityBySearch}"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;option value="${authority.authorityId }" selected="selected"&gt;${authority.authorityName }&lt;/option&gt;</t>
+  </si>
+  <si>
+    <t>&lt;c:set var="printAuthorityFlag" value="0"/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;/c:when&gt;</t>
+  </si>
+  <si>
+    <t>&lt;/c:choose&gt;</t>
+  </si>
+  <si>
+    <t>&lt;/c:forEach&gt;</t>
+  </si>
+  <si>
+    <t>&lt;c:if test="${ printAuthorityFlag eq '1' }"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;option value="${authority.authorityId }"&gt;${authority.authorityName }&lt;/option&gt;</t>
+  </si>
+  <si>
+    <t>&lt;/c:if&gt;</t>
+  </si>
+  <si>
+    <t>&lt;c:otherwise&gt;</t>
+  </si>
+  <si>
+    <t>&lt;/c:otherwise&gt;</t>
+  </si>
+  <si>
+    <t>&lt;/select&gt;</t>
+  </si>
+  <si>
+    <t>sys0501.jsp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>private List&lt;Integer&gt; authorityId = new ArrayList&lt;Integer&gt;();</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -373,8 +511,17 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -390,6 +537,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -501,7 +666,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -516,29 +681,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -558,6 +701,41 @@
     <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1211,6 +1389,424 @@
             <a:t>)</a:t>
           </a:r>
           <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>666750</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="矩形 3"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3990975" y="5514975"/>
+          <a:ext cx="790575" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="矩形标注 4"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6210300" y="4962525"/>
+          <a:ext cx="2085975" cy="819150"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -115353"/>
+            <a:gd name="adj2" fmla="val 24128"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1400"/>
+            <a:t>Timestamp</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1400"/>
+            <a:t>为固定后缀</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1400"/>
+            <a:t>,</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1400"/>
+            <a:t>为了时间控件的隐藏域使用</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="矩形标注 5"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9601200" y="8067675"/>
+          <a:ext cx="2057400" cy="857250"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -94915"/>
+            <a:gd name="adj2" fmla="val 119571"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
+            <a:t>检索后</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
+            <a:t>,</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
+            <a:t>多选框有数据时恢复选中状态</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
+            <a:t>(</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
+            <a:t>检索后检索条件保持使用</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
+            <a:t>)</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="圆角矩形标注 6"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="876300" y="9477375"/>
+          <a:ext cx="2276475" cy="752475"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRoundRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 54843"/>
+            <a:gd name="adj2" fmla="val -81656"/>
+            <a:gd name="adj3" fmla="val 16667"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
+            <a:t>外层循环时，对内层循环做一个标记动作，防止内层循环多次循环造成数据重复</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="矩形标注 7"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12458700" y="11630025"/>
+          <a:ext cx="2762250" cy="695325"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -57738"/>
+            <a:gd name="adj2" fmla="val -179392"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
+            <a:t>循环检索后的检索条件</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
+            <a:t>,</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
+            <a:t>两者相同时赋予选中状态</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
+            <a:t>,</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
+            <a:t>内层循环标记设置为</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
+            <a:t>0,</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
+            <a:t>禁止本次外循环打印数据</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>76</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="矩形标注 8"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10344150" y="12353925"/>
+          <a:ext cx="1905000" cy="628650"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -20333"/>
+            <a:gd name="adj2" fmla="val -189015"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
+            <a:t>内层循环没有打印时进行本次外层循环的打印数据</a:t>
+          </a:r>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -1509,10 +2105,10 @@
   <sheetPr>
     <tabColor rgb="FF002060"/>
   </sheetPr>
-  <dimension ref="A1:P21"/>
+  <dimension ref="A1:P29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1524,20 +2120,20 @@
       <c r="A1" s="3"/>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
       <c r="J1" s="3"/>
       <c r="K1" s="3"/>
       <c r="L1" s="3"/>
       <c r="M1" s="3"/>
       <c r="N1" s="3"/>
-      <c r="O1" s="10" t="s">
+      <c r="O1" s="26" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1547,81 +2143,81 @@
       <c r="C2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="27"/>
       <c r="J2" s="3"/>
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
       <c r="N2" s="3"/>
-      <c r="O2" s="10"/>
+      <c r="O2" s="26"/>
       <c r="P2" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14"/>
-      <c r="K3" s="14"/>
-      <c r="L3" s="14"/>
-      <c r="M3" s="14"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
+      <c r="H3" s="30"/>
+      <c r="I3" s="30"/>
+      <c r="J3" s="30"/>
+      <c r="K3" s="30"/>
+      <c r="L3" s="30"/>
+      <c r="M3" s="30"/>
       <c r="O3" s="2"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="14"/>
-      <c r="J4" s="14"/>
-      <c r="K4" s="14"/>
-      <c r="L4" s="14"/>
-      <c r="M4" s="14"/>
+      <c r="B4" s="30"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="30"/>
+      <c r="I4" s="30"/>
+      <c r="J4" s="30"/>
+      <c r="K4" s="30"/>
+      <c r="L4" s="30"/>
+      <c r="M4" s="30"/>
       <c r="O4" s="6">
         <v>101</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="13"/>
+      <c r="C5" s="29"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="C6" s="13" t="s">
+      <c r="C6" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="13"/>
+      <c r="D6" s="29"/>
+      <c r="E6" s="29"/>
+      <c r="F6" s="29"/>
+      <c r="G6" s="29"/>
+      <c r="H6" s="29"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="13"/>
+      <c r="D7" s="29"/>
+      <c r="E7" s="29"/>
+      <c r="F7" s="29"/>
+      <c r="G7" s="29"/>
+      <c r="H7" s="29"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.15">
       <c r="C8" s="5">
@@ -1656,30 +2252,30 @@
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="D14" s="12" t="s">
+      <c r="D14" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="12"/>
-      <c r="J14" s="12"/>
-      <c r="K14" s="12"/>
-      <c r="L14" s="12"/>
-      <c r="M14" s="12"/>
+      <c r="E14" s="28"/>
+      <c r="F14" s="28"/>
+      <c r="G14" s="28"/>
+      <c r="H14" s="28"/>
+      <c r="I14" s="28"/>
+      <c r="J14" s="28"/>
+      <c r="K14" s="28"/>
+      <c r="L14" s="28"/>
+      <c r="M14" s="28"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="12"/>
-      <c r="J15" s="12"/>
-      <c r="K15" s="12"/>
-      <c r="L15" s="12"/>
-      <c r="M15" s="12"/>
+      <c r="D15" s="28"/>
+      <c r="E15" s="28"/>
+      <c r="F15" s="28"/>
+      <c r="G15" s="28"/>
+      <c r="H15" s="28"/>
+      <c r="I15" s="28"/>
+      <c r="J15" s="28"/>
+      <c r="K15" s="28"/>
+      <c r="L15" s="28"/>
+      <c r="M15" s="28"/>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B17" t="s">
@@ -1687,35 +2283,88 @@
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.15">
-      <c r="C18" s="32" t="s">
+      <c r="C18" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="D18" s="32" t="s">
+      <c r="D18" s="24" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.15">
-      <c r="C19" s="33" t="s">
+      <c r="C19" s="25" t="s">
         <v>58</v>
       </c>
-      <c r="D19" s="33">
+      <c r="D19" s="25">
         <v>5</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.15">
-      <c r="C20" s="33" t="s">
+      <c r="C20" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="D20" s="33">
+      <c r="D20" s="25">
         <v>9</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.15">
-      <c r="C21" s="33" t="s">
+      <c r="C21" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="D21" s="33">
+      <c r="D21" s="25">
         <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="B23" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="C24" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="D24" s="24" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="C25" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="D25" s="25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="C26" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="D26" s="25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="C27" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="D27" s="25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="C28" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="D28" s="25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="C29" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="D29" s="25">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -1749,13 +2398,13 @@
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B6" s="9" t="s">
@@ -1764,16 +2413,16 @@
       <c r="C6" s="9"/>
     </row>
     <row r="82" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A82" s="17" t="s">
+      <c r="A82" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="B82" s="17"/>
+      <c r="B82" s="32"/>
     </row>
     <row r="83" spans="1:14" x14ac:dyDescent="0.15">
       <c r="B83" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C83" s="18" t="s">
+      <c r="C83" s="33" t="s">
         <v>24</v>
       </c>
       <c r="D83" s="8" t="s">
@@ -1784,7 +2433,7 @@
       <c r="G83" s="8"/>
       <c r="H83" s="8"/>
       <c r="I83" s="8"/>
-      <c r="J83" s="18" t="s">
+      <c r="J83" s="33" t="s">
         <v>25</v>
       </c>
       <c r="K83" s="8" t="s">
@@ -1795,7 +2444,7 @@
       <c r="N83" s="8"/>
     </row>
     <row r="84" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="C84" s="18"/>
+      <c r="C84" s="33"/>
       <c r="D84" s="8" t="s">
         <v>19</v>
       </c>
@@ -1804,14 +2453,14 @@
       <c r="G84" s="8"/>
       <c r="H84" s="8"/>
       <c r="I84" s="8"/>
-      <c r="J84" s="18"/>
+      <c r="J84" s="33"/>
       <c r="K84" s="8" t="s">
         <v>19</v>
       </c>
       <c r="L84" s="8"/>
     </row>
     <row r="85" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="C85" s="18"/>
+      <c r="C85" s="33"/>
       <c r="D85" s="8"/>
       <c r="E85" s="8" t="s">
         <v>20</v>
@@ -1820,14 +2469,14 @@
       <c r="G85" s="8"/>
       <c r="H85" s="8"/>
       <c r="I85" s="8"/>
-      <c r="J85" s="18"/>
+      <c r="J85" s="33"/>
       <c r="K85" s="8"/>
       <c r="L85" s="8" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="86" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="C86" s="18"/>
+      <c r="C86" s="33"/>
       <c r="D86" s="8"/>
       <c r="E86" s="8" t="s">
         <v>21</v>
@@ -1836,14 +2485,14 @@
       <c r="G86" s="8"/>
       <c r="H86" s="8"/>
       <c r="I86" s="8"/>
-      <c r="J86" s="18"/>
+      <c r="J86" s="33"/>
       <c r="K86" s="8"/>
       <c r="L86" s="8" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="87" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="C87" s="18"/>
+      <c r="C87" s="33"/>
       <c r="D87" s="8"/>
       <c r="E87" s="8" t="s">
         <v>26</v>
@@ -1852,14 +2501,14 @@
       <c r="G87" s="8"/>
       <c r="H87" s="8"/>
       <c r="I87" s="8"/>
-      <c r="J87" s="18"/>
+      <c r="J87" s="33"/>
       <c r="K87" s="8"/>
       <c r="L87" s="8" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="88" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="C88" s="18"/>
+      <c r="C88" s="33"/>
       <c r="D88" s="8" t="s">
         <v>23</v>
       </c>
@@ -1868,75 +2517,75 @@
       <c r="G88" s="8"/>
       <c r="H88" s="8"/>
       <c r="I88" s="8"/>
-      <c r="J88" s="18"/>
+      <c r="J88" s="33"/>
       <c r="K88" s="8" t="s">
         <v>23</v>
       </c>
       <c r="L88" s="8"/>
     </row>
     <row r="89" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="C89" s="18"/>
+      <c r="C89" s="33"/>
       <c r="D89" s="8"/>
-      <c r="J89" s="18"/>
+      <c r="J89" s="33"/>
     </row>
     <row r="90" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="C90" s="18"/>
-      <c r="J90" s="18"/>
+      <c r="C90" s="33"/>
+      <c r="J90" s="33"/>
     </row>
     <row r="91" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="C91" s="18"/>
-      <c r="J91" s="18"/>
+      <c r="C91" s="33"/>
+      <c r="J91" s="33"/>
     </row>
     <row r="92" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="C92" s="18"/>
-      <c r="J92" s="18"/>
+      <c r="C92" s="33"/>
+      <c r="J92" s="33"/>
     </row>
     <row r="93" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A93" s="16" t="s">
+      <c r="A93" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="B93" s="16"/>
-      <c r="C93" s="18"/>
+      <c r="B93" s="34"/>
+      <c r="C93" s="33"/>
       <c r="D93" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="J93" s="18"/>
+      <c r="J93" s="33"/>
       <c r="K93" s="8" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="94" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="C94" s="18"/>
+      <c r="C94" s="33"/>
       <c r="D94" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="J94" s="18"/>
+      <c r="J94" s="33"/>
       <c r="K94" s="8" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="95" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="C95" s="18"/>
-      <c r="J95" s="18"/>
+      <c r="C95" s="33"/>
+      <c r="J95" s="33"/>
     </row>
     <row r="96" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="C96" s="18"/>
-      <c r="J96" s="18"/>
+      <c r="C96" s="33"/>
+      <c r="J96" s="33"/>
     </row>
     <row r="97" spans="3:10" x14ac:dyDescent="0.15">
-      <c r="C97" s="18"/>
-      <c r="J97" s="18"/>
+      <c r="C97" s="33"/>
+      <c r="J97" s="33"/>
     </row>
     <row r="98" spans="3:10" x14ac:dyDescent="0.15">
-      <c r="C98" s="18"/>
-      <c r="J98" s="18"/>
+      <c r="C98" s="33"/>
+      <c r="J98" s="33"/>
     </row>
     <row r="99" spans="3:10" x14ac:dyDescent="0.15">
-      <c r="C99" s="18"/>
-      <c r="J99" s="18"/>
+      <c r="C99" s="33"/>
+      <c r="J99" s="33"/>
     </row>
     <row r="100" spans="3:10" x14ac:dyDescent="0.15">
-      <c r="J100" s="18"/>
+      <c r="J100" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -1955,640 +2604,1962 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S28"/>
+  <dimension ref="A1:W80"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="D1" s="11" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22" t="s">
+      <c r="C2" s="14"/>
+      <c r="D2" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22"/>
-      <c r="I2" s="22"/>
-      <c r="J2" s="22"/>
-      <c r="K2" s="22"/>
-      <c r="L2" s="22"/>
-      <c r="M2" s="22"/>
-      <c r="N2" s="22"/>
-      <c r="O2" s="22"/>
-      <c r="P2" s="22"/>
-      <c r="Q2" s="22"/>
-      <c r="R2" s="22"/>
-      <c r="S2" s="23"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="14"/>
+      <c r="M2" s="14"/>
+      <c r="N2" s="14"/>
+      <c r="O2" s="14"/>
+      <c r="P2" s="14"/>
+      <c r="Q2" s="14"/>
+      <c r="R2" s="14"/>
+      <c r="S2" s="15"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A3" s="24"/>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25" t="s">
+      <c r="A3" s="16"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
-      <c r="K3" s="25"/>
-      <c r="L3" s="25"/>
-      <c r="M3" s="25"/>
-      <c r="N3" s="25"/>
-      <c r="O3" s="25"/>
-      <c r="P3" s="25"/>
-      <c r="Q3" s="25"/>
-      <c r="R3" s="25"/>
-      <c r="S3" s="26"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="17"/>
+      <c r="K3" s="17"/>
+      <c r="L3" s="17"/>
+      <c r="M3" s="17"/>
+      <c r="N3" s="17"/>
+      <c r="O3" s="17"/>
+      <c r="P3" s="17"/>
+      <c r="Q3" s="17"/>
+      <c r="R3" s="17"/>
+      <c r="S3" s="18"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A4" s="24"/>
-      <c r="B4" s="25"/>
-      <c r="C4" s="25"/>
-      <c r="D4" s="25" t="s">
+      <c r="A4" s="16"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="E4" s="25"/>
-      <c r="F4" s="25"/>
-      <c r="G4" s="25"/>
-      <c r="H4" s="25"/>
-      <c r="I4" s="25"/>
-      <c r="J4" s="25"/>
-      <c r="K4" s="25"/>
-      <c r="L4" s="25"/>
-      <c r="M4" s="25"/>
-      <c r="N4" s="25"/>
-      <c r="O4" s="25"/>
-      <c r="P4" s="25"/>
-      <c r="Q4" s="25"/>
-      <c r="R4" s="25"/>
-      <c r="S4" s="26"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
+      <c r="J4" s="17"/>
+      <c r="K4" s="17"/>
+      <c r="L4" s="17"/>
+      <c r="M4" s="17"/>
+      <c r="N4" s="17"/>
+      <c r="O4" s="17"/>
+      <c r="P4" s="17"/>
+      <c r="Q4" s="17"/>
+      <c r="R4" s="17"/>
+      <c r="S4" s="18"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A5" s="24"/>
-      <c r="B5" s="25"/>
-      <c r="C5" s="25"/>
-      <c r="D5" s="25"/>
-      <c r="E5" s="25" t="s">
+      <c r="A5" s="16"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="F5" s="25"/>
-      <c r="G5" s="25"/>
-      <c r="H5" s="25"/>
-      <c r="I5" s="25"/>
-      <c r="J5" s="25"/>
-      <c r="K5" s="25"/>
-      <c r="L5" s="25"/>
-      <c r="M5" s="25"/>
-      <c r="N5" s="25"/>
-      <c r="O5" s="25"/>
-      <c r="P5" s="25"/>
-      <c r="Q5" s="25"/>
-      <c r="R5" s="25"/>
-      <c r="S5" s="26"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="17"/>
+      <c r="J5" s="17"/>
+      <c r="K5" s="17"/>
+      <c r="L5" s="17"/>
+      <c r="M5" s="17"/>
+      <c r="N5" s="17"/>
+      <c r="O5" s="17"/>
+      <c r="P5" s="17"/>
+      <c r="Q5" s="17"/>
+      <c r="R5" s="17"/>
+      <c r="S5" s="18"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A6" s="24"/>
-      <c r="B6" s="25"/>
-      <c r="C6" s="25"/>
-      <c r="D6" s="25" t="s">
+      <c r="A6" s="16"/>
+      <c r="B6" s="17"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="E6" s="25"/>
-      <c r="F6" s="25"/>
-      <c r="G6" s="25"/>
-      <c r="H6" s="25"/>
-      <c r="I6" s="25"/>
-      <c r="J6" s="25"/>
-      <c r="K6" s="25"/>
-      <c r="L6" s="25"/>
-      <c r="M6" s="25"/>
-      <c r="N6" s="25"/>
-      <c r="O6" s="25"/>
-      <c r="P6" s="25"/>
-      <c r="Q6" s="25"/>
-      <c r="R6" s="25"/>
-      <c r="S6" s="26"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="17"/>
+      <c r="J6" s="17"/>
+      <c r="K6" s="17"/>
+      <c r="L6" s="17"/>
+      <c r="M6" s="17"/>
+      <c r="N6" s="17"/>
+      <c r="O6" s="17"/>
+      <c r="P6" s="17"/>
+      <c r="Q6" s="17"/>
+      <c r="R6" s="17"/>
+      <c r="S6" s="18"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A7" s="24"/>
-      <c r="B7" s="25"/>
-      <c r="C7" s="25"/>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25" t="s">
+      <c r="A7" s="16"/>
+      <c r="B7" s="17"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="F7" s="25"/>
-      <c r="G7" s="25"/>
-      <c r="H7" s="25"/>
-      <c r="I7" s="25"/>
-      <c r="J7" s="25"/>
-      <c r="K7" s="25"/>
-      <c r="L7" s="25"/>
-      <c r="M7" s="25"/>
-      <c r="N7" s="25"/>
-      <c r="O7" s="25"/>
-      <c r="P7" s="25"/>
-      <c r="Q7" s="25"/>
-      <c r="R7" s="25"/>
-      <c r="S7" s="26"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="17"/>
+      <c r="I7" s="17"/>
+      <c r="J7" s="17"/>
+      <c r="K7" s="17"/>
+      <c r="L7" s="17"/>
+      <c r="M7" s="17"/>
+      <c r="N7" s="17"/>
+      <c r="O7" s="17"/>
+      <c r="P7" s="17"/>
+      <c r="Q7" s="17"/>
+      <c r="R7" s="17"/>
+      <c r="S7" s="18"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A8" s="24"/>
-      <c r="B8" s="25"/>
-      <c r="C8" s="25"/>
-      <c r="D8" s="25"/>
-      <c r="E8" s="25" t="s">
+      <c r="A8" s="16"/>
+      <c r="B8" s="17"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="F8" s="25"/>
-      <c r="G8" s="25"/>
-      <c r="H8" s="25"/>
-      <c r="I8" s="25"/>
-      <c r="J8" s="25"/>
-      <c r="K8" s="25"/>
-      <c r="L8" s="25"/>
-      <c r="M8" s="25"/>
-      <c r="N8" s="25"/>
-      <c r="O8" s="25"/>
-      <c r="P8" s="25"/>
-      <c r="Q8" s="25"/>
-      <c r="R8" s="25"/>
-      <c r="S8" s="26"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="17"/>
+      <c r="J8" s="17"/>
+      <c r="K8" s="17"/>
+      <c r="L8" s="17"/>
+      <c r="M8" s="17"/>
+      <c r="N8" s="17"/>
+      <c r="O8" s="17"/>
+      <c r="P8" s="17"/>
+      <c r="Q8" s="17"/>
+      <c r="R8" s="17"/>
+      <c r="S8" s="18"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A9" s="24"/>
-      <c r="B9" s="25"/>
-      <c r="C9" s="25"/>
-      <c r="D9" s="25" t="s">
+      <c r="A9" s="16"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="E9" s="25"/>
-      <c r="F9" s="25"/>
-      <c r="G9" s="25"/>
-      <c r="H9" s="25"/>
-      <c r="I9" s="25"/>
-      <c r="J9" s="25"/>
-      <c r="K9" s="25"/>
-      <c r="L9" s="25"/>
-      <c r="M9" s="25"/>
-      <c r="N9" s="25"/>
-      <c r="O9" s="25"/>
-      <c r="P9" s="25"/>
-      <c r="Q9" s="25"/>
-      <c r="R9" s="25"/>
-      <c r="S9" s="26"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="17"/>
+      <c r="J9" s="17"/>
+      <c r="K9" s="17"/>
+      <c r="L9" s="17"/>
+      <c r="M9" s="17"/>
+      <c r="N9" s="17"/>
+      <c r="O9" s="17"/>
+      <c r="P9" s="17"/>
+      <c r="Q9" s="17"/>
+      <c r="R9" s="17"/>
+      <c r="S9" s="18"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A10" s="24"/>
-      <c r="B10" s="25"/>
-      <c r="C10" s="25"/>
-      <c r="D10" s="25" t="s">
+      <c r="A10" s="16"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="E10" s="25"/>
-      <c r="F10" s="25"/>
-      <c r="G10" s="25"/>
-      <c r="H10" s="25"/>
-      <c r="I10" s="25"/>
-      <c r="J10" s="25"/>
-      <c r="K10" s="25"/>
-      <c r="L10" s="25"/>
-      <c r="M10" s="25"/>
-      <c r="N10" s="25"/>
-      <c r="O10" s="25"/>
-      <c r="P10" s="25"/>
-      <c r="Q10" s="25"/>
-      <c r="R10" s="25"/>
-      <c r="S10" s="26"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="17"/>
+      <c r="J10" s="17"/>
+      <c r="K10" s="17"/>
+      <c r="L10" s="17"/>
+      <c r="M10" s="17"/>
+      <c r="N10" s="17"/>
+      <c r="O10" s="17"/>
+      <c r="P10" s="17"/>
+      <c r="Q10" s="17"/>
+      <c r="R10" s="17"/>
+      <c r="S10" s="18"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A11" s="24"/>
-      <c r="B11" s="25"/>
-      <c r="C11" s="25"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="25"/>
-      <c r="F11" s="25"/>
-      <c r="G11" s="25"/>
-      <c r="H11" s="25"/>
-      <c r="I11" s="25"/>
-      <c r="J11" s="25"/>
-      <c r="K11" s="25"/>
-      <c r="L11" s="25"/>
-      <c r="M11" s="25"/>
-      <c r="N11" s="25"/>
-      <c r="O11" s="25"/>
-      <c r="P11" s="25"/>
-      <c r="Q11" s="25"/>
-      <c r="R11" s="25"/>
-      <c r="S11" s="26"/>
+      <c r="A11" s="16"/>
+      <c r="B11" s="17"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="17"/>
+      <c r="I11" s="17"/>
+      <c r="J11" s="17"/>
+      <c r="K11" s="17"/>
+      <c r="L11" s="17"/>
+      <c r="M11" s="17"/>
+      <c r="N11" s="17"/>
+      <c r="O11" s="17"/>
+      <c r="P11" s="17"/>
+      <c r="Q11" s="17"/>
+      <c r="R11" s="17"/>
+      <c r="S11" s="18"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A12" s="24"/>
-      <c r="B12" s="25" t="s">
+      <c r="A12" s="16"/>
+      <c r="B12" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="C12" s="25"/>
-      <c r="D12" s="25" t="s">
+      <c r="C12" s="17"/>
+      <c r="D12" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="E12" s="25"/>
-      <c r="F12" s="25"/>
-      <c r="G12" s="25"/>
-      <c r="H12" s="25"/>
-      <c r="I12" s="25"/>
-      <c r="J12" s="25"/>
-      <c r="K12" s="25"/>
-      <c r="L12" s="25"/>
-      <c r="M12" s="25"/>
-      <c r="N12" s="25"/>
-      <c r="O12" s="25"/>
-      <c r="P12" s="25"/>
-      <c r="Q12" s="25"/>
-      <c r="R12" s="25"/>
-      <c r="S12" s="26"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="17"/>
+      <c r="H12" s="17"/>
+      <c r="I12" s="17"/>
+      <c r="J12" s="17"/>
+      <c r="K12" s="17"/>
+      <c r="L12" s="17"/>
+      <c r="M12" s="17"/>
+      <c r="N12" s="17"/>
+      <c r="O12" s="17"/>
+      <c r="P12" s="17"/>
+      <c r="Q12" s="17"/>
+      <c r="R12" s="17"/>
+      <c r="S12" s="18"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A13" s="24"/>
-      <c r="B13" s="25"/>
-      <c r="C13" s="25"/>
-      <c r="D13" s="25" t="s">
+      <c r="A13" s="16"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="E13" s="25"/>
-      <c r="F13" s="25"/>
-      <c r="G13" s="25"/>
-      <c r="H13" s="25"/>
-      <c r="I13" s="25"/>
-      <c r="J13" s="25"/>
-      <c r="K13" s="25"/>
-      <c r="L13" s="25"/>
-      <c r="M13" s="25"/>
-      <c r="N13" s="25"/>
-      <c r="O13" s="25"/>
-      <c r="P13" s="25"/>
-      <c r="Q13" s="25"/>
-      <c r="R13" s="25"/>
-      <c r="S13" s="26"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="17"/>
+      <c r="H13" s="17"/>
+      <c r="I13" s="17"/>
+      <c r="J13" s="17"/>
+      <c r="K13" s="17"/>
+      <c r="L13" s="17"/>
+      <c r="M13" s="17"/>
+      <c r="N13" s="17"/>
+      <c r="O13" s="17"/>
+      <c r="P13" s="17"/>
+      <c r="Q13" s="17"/>
+      <c r="R13" s="17"/>
+      <c r="S13" s="18"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A14" s="24"/>
-      <c r="B14" s="25"/>
-      <c r="C14" s="25"/>
-      <c r="D14" s="25" t="s">
+      <c r="A14" s="16"/>
+      <c r="B14" s="17"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="E14" s="25"/>
-      <c r="F14" s="25"/>
-      <c r="G14" s="25"/>
-      <c r="H14" s="25"/>
-      <c r="I14" s="25"/>
-      <c r="J14" s="25"/>
-      <c r="K14" s="25"/>
-      <c r="L14" s="25"/>
-      <c r="M14" s="25"/>
-      <c r="N14" s="25"/>
-      <c r="O14" s="25"/>
-      <c r="P14" s="25"/>
-      <c r="Q14" s="25"/>
-      <c r="R14" s="25"/>
-      <c r="S14" s="26"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="17"/>
+      <c r="H14" s="17"/>
+      <c r="I14" s="17"/>
+      <c r="J14" s="17"/>
+      <c r="K14" s="17"/>
+      <c r="L14" s="17"/>
+      <c r="M14" s="17"/>
+      <c r="N14" s="17"/>
+      <c r="O14" s="17"/>
+      <c r="P14" s="17"/>
+      <c r="Q14" s="17"/>
+      <c r="R14" s="17"/>
+      <c r="S14" s="18"/>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A15" s="24"/>
-      <c r="B15" s="25"/>
-      <c r="C15" s="25"/>
-      <c r="D15" s="25"/>
-      <c r="E15" s="25" t="s">
+      <c r="A15" s="16"/>
+      <c r="B15" s="17"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="F15" s="25"/>
-      <c r="G15" s="25"/>
-      <c r="H15" s="25"/>
-      <c r="I15" s="25"/>
-      <c r="J15" s="25"/>
-      <c r="K15" s="25"/>
-      <c r="L15" s="25"/>
-      <c r="M15" s="25"/>
-      <c r="N15" s="25"/>
-      <c r="O15" s="25"/>
-      <c r="P15" s="25"/>
-      <c r="Q15" s="25"/>
-      <c r="R15" s="25"/>
-      <c r="S15" s="26"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="17"/>
+      <c r="I15" s="17"/>
+      <c r="J15" s="17"/>
+      <c r="K15" s="17"/>
+      <c r="L15" s="17"/>
+      <c r="M15" s="17"/>
+      <c r="N15" s="17"/>
+      <c r="O15" s="17"/>
+      <c r="P15" s="17"/>
+      <c r="Q15" s="17"/>
+      <c r="R15" s="17"/>
+      <c r="S15" s="18"/>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A16" s="24"/>
-      <c r="B16" s="25"/>
-      <c r="C16" s="25"/>
-      <c r="D16" s="25"/>
-      <c r="E16" s="25" t="s">
+      <c r="A16" s="16"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="F16" s="25"/>
-      <c r="G16" s="25"/>
-      <c r="H16" s="25"/>
-      <c r="I16" s="25"/>
-      <c r="J16" s="25"/>
-      <c r="K16" s="25"/>
-      <c r="L16" s="25"/>
-      <c r="M16" s="25"/>
-      <c r="N16" s="25"/>
-      <c r="O16" s="25"/>
-      <c r="P16" s="25"/>
-      <c r="Q16" s="25"/>
-      <c r="R16" s="25"/>
-      <c r="S16" s="26"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="17"/>
+      <c r="I16" s="17"/>
+      <c r="J16" s="17"/>
+      <c r="K16" s="17"/>
+      <c r="L16" s="17"/>
+      <c r="M16" s="17"/>
+      <c r="N16" s="17"/>
+      <c r="O16" s="17"/>
+      <c r="P16" s="17"/>
+      <c r="Q16" s="17"/>
+      <c r="R16" s="17"/>
+      <c r="S16" s="18"/>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A17" s="24"/>
-      <c r="B17" s="25"/>
-      <c r="C17" s="25"/>
-      <c r="D17" s="25" t="s">
+      <c r="A17" s="16"/>
+      <c r="B17" s="17"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="E17" s="25"/>
-      <c r="F17" s="25"/>
-      <c r="G17" s="25"/>
-      <c r="H17" s="25"/>
-      <c r="I17" s="25"/>
-      <c r="J17" s="25"/>
-      <c r="K17" s="25"/>
-      <c r="L17" s="25"/>
-      <c r="M17" s="25"/>
-      <c r="N17" s="25"/>
-      <c r="O17" s="25"/>
-      <c r="P17" s="25"/>
-      <c r="Q17" s="25"/>
-      <c r="R17" s="25"/>
-      <c r="S17" s="26"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="17"/>
+      <c r="G17" s="17"/>
+      <c r="H17" s="17"/>
+      <c r="I17" s="17"/>
+      <c r="J17" s="17"/>
+      <c r="K17" s="17"/>
+      <c r="L17" s="17"/>
+      <c r="M17" s="17"/>
+      <c r="N17" s="17"/>
+      <c r="O17" s="17"/>
+      <c r="P17" s="17"/>
+      <c r="Q17" s="17"/>
+      <c r="R17" s="17"/>
+      <c r="S17" s="18"/>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A18" s="24"/>
-      <c r="B18" s="25"/>
-      <c r="C18" s="25"/>
-      <c r="D18" s="25" t="s">
+      <c r="A18" s="16"/>
+      <c r="B18" s="17"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="E18" s="25"/>
-      <c r="F18" s="25"/>
-      <c r="G18" s="25"/>
-      <c r="H18" s="25"/>
-      <c r="I18" s="25"/>
-      <c r="J18" s="25"/>
-      <c r="K18" s="25"/>
-      <c r="L18" s="25"/>
-      <c r="M18" s="25"/>
-      <c r="N18" s="25"/>
-      <c r="O18" s="25"/>
-      <c r="P18" s="25"/>
-      <c r="Q18" s="25"/>
-      <c r="R18" s="25"/>
-      <c r="S18" s="26"/>
+      <c r="E18" s="17"/>
+      <c r="F18" s="17"/>
+      <c r="G18" s="17"/>
+      <c r="H18" s="17"/>
+      <c r="I18" s="17"/>
+      <c r="J18" s="17"/>
+      <c r="K18" s="17"/>
+      <c r="L18" s="17"/>
+      <c r="M18" s="17"/>
+      <c r="N18" s="17"/>
+      <c r="O18" s="17"/>
+      <c r="P18" s="17"/>
+      <c r="Q18" s="17"/>
+      <c r="R18" s="17"/>
+      <c r="S18" s="18"/>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A19" s="24"/>
-      <c r="B19" s="25"/>
-      <c r="C19" s="25"/>
-      <c r="D19" s="25"/>
-      <c r="E19" s="25" t="s">
+      <c r="A19" s="16"/>
+      <c r="B19" s="17"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="F19" s="25"/>
-      <c r="G19" s="25"/>
-      <c r="H19" s="25"/>
-      <c r="I19" s="25"/>
-      <c r="J19" s="25"/>
-      <c r="K19" s="25"/>
-      <c r="L19" s="25"/>
-      <c r="M19" s="25"/>
-      <c r="N19" s="25"/>
-      <c r="O19" s="25"/>
-      <c r="P19" s="25"/>
-      <c r="Q19" s="25"/>
-      <c r="R19" s="25"/>
-      <c r="S19" s="26"/>
+      <c r="F19" s="17"/>
+      <c r="G19" s="17"/>
+      <c r="H19" s="17"/>
+      <c r="I19" s="17"/>
+      <c r="J19" s="17"/>
+      <c r="K19" s="17"/>
+      <c r="L19" s="17"/>
+      <c r="M19" s="17"/>
+      <c r="N19" s="17"/>
+      <c r="O19" s="17"/>
+      <c r="P19" s="17"/>
+      <c r="Q19" s="17"/>
+      <c r="R19" s="17"/>
+      <c r="S19" s="18"/>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A20" s="24"/>
-      <c r="B20" s="25"/>
-      <c r="C20" s="25"/>
-      <c r="D20" s="25"/>
-      <c r="E20" s="25"/>
-      <c r="F20" s="25" t="s">
+      <c r="A20" s="16"/>
+      <c r="B20" s="17"/>
+      <c r="C20" s="17"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="17"/>
+      <c r="F20" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="G20" s="25"/>
-      <c r="H20" s="25"/>
-      <c r="I20" s="25"/>
-      <c r="J20" s="25"/>
-      <c r="K20" s="25"/>
-      <c r="L20" s="30"/>
-      <c r="M20" s="30"/>
-      <c r="N20" s="30"/>
-      <c r="O20" s="30"/>
-      <c r="P20" s="30"/>
-      <c r="Q20" s="25"/>
-      <c r="R20" s="25"/>
-      <c r="S20" s="26"/>
+      <c r="G20" s="17"/>
+      <c r="H20" s="17"/>
+      <c r="I20" s="17"/>
+      <c r="J20" s="17"/>
+      <c r="K20" s="17"/>
+      <c r="L20" s="22"/>
+      <c r="M20" s="22"/>
+      <c r="N20" s="22"/>
+      <c r="O20" s="22"/>
+      <c r="P20" s="22"/>
+      <c r="Q20" s="17"/>
+      <c r="R20" s="17"/>
+      <c r="S20" s="18"/>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A21" s="24"/>
-      <c r="B21" s="25"/>
-      <c r="C21" s="25"/>
-      <c r="D21" s="25"/>
-      <c r="E21" s="30" t="s">
+      <c r="A21" s="16"/>
+      <c r="B21" s="17"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="F21" s="31"/>
-      <c r="G21" s="31"/>
-      <c r="H21" s="31"/>
-      <c r="I21" s="31"/>
-      <c r="J21" s="25"/>
-      <c r="K21" s="25"/>
-      <c r="L21" s="25"/>
-      <c r="M21" s="25"/>
-      <c r="N21" s="25"/>
-      <c r="O21" s="25"/>
-      <c r="P21" s="25"/>
-      <c r="Q21" s="25"/>
-      <c r="R21" s="25"/>
-      <c r="S21" s="26"/>
+      <c r="F21" s="23"/>
+      <c r="G21" s="23"/>
+      <c r="H21" s="23"/>
+      <c r="I21" s="23"/>
+      <c r="J21" s="17"/>
+      <c r="K21" s="17"/>
+      <c r="L21" s="17"/>
+      <c r="M21" s="17"/>
+      <c r="N21" s="17"/>
+      <c r="O21" s="17"/>
+      <c r="P21" s="17"/>
+      <c r="Q21" s="17"/>
+      <c r="R21" s="17"/>
+      <c r="S21" s="18"/>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A22" s="24"/>
-      <c r="B22" s="25"/>
-      <c r="C22" s="25"/>
-      <c r="D22" s="25" t="s">
+      <c r="A22" s="16"/>
+      <c r="B22" s="17"/>
+      <c r="C22" s="17"/>
+      <c r="D22" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="E22" s="25"/>
-      <c r="F22" s="25"/>
-      <c r="G22" s="25"/>
-      <c r="H22" s="25"/>
-      <c r="I22" s="25"/>
-      <c r="J22" s="25"/>
-      <c r="K22" s="25"/>
-      <c r="L22" s="25"/>
-      <c r="M22" s="25"/>
-      <c r="N22" s="25"/>
-      <c r="O22" s="25"/>
-      <c r="P22" s="25"/>
-      <c r="Q22" s="25"/>
-      <c r="R22" s="25"/>
-      <c r="S22" s="26"/>
+      <c r="E22" s="17"/>
+      <c r="F22" s="17"/>
+      <c r="G22" s="17"/>
+      <c r="H22" s="17"/>
+      <c r="I22" s="17"/>
+      <c r="J22" s="17"/>
+      <c r="K22" s="17"/>
+      <c r="L22" s="17"/>
+      <c r="M22" s="17"/>
+      <c r="N22" s="17"/>
+      <c r="O22" s="17"/>
+      <c r="P22" s="17"/>
+      <c r="Q22" s="17"/>
+      <c r="R22" s="17"/>
+      <c r="S22" s="18"/>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A23" s="24"/>
-      <c r="B23" s="25"/>
-      <c r="C23" s="25"/>
-      <c r="D23" s="25" t="s">
+      <c r="A23" s="16"/>
+      <c r="B23" s="17"/>
+      <c r="C23" s="17"/>
+      <c r="D23" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="E23" s="25"/>
-      <c r="F23" s="25"/>
-      <c r="G23" s="25"/>
-      <c r="H23" s="25"/>
-      <c r="I23" s="25"/>
-      <c r="J23" s="25"/>
-      <c r="K23" s="25"/>
-      <c r="L23" s="25"/>
-      <c r="M23" s="25"/>
-      <c r="N23" s="25"/>
-      <c r="O23" s="25"/>
-      <c r="P23" s="25"/>
-      <c r="Q23" s="25"/>
-      <c r="R23" s="25"/>
-      <c r="S23" s="26"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="17"/>
+      <c r="G23" s="17"/>
+      <c r="H23" s="17"/>
+      <c r="I23" s="17"/>
+      <c r="J23" s="17"/>
+      <c r="K23" s="17"/>
+      <c r="L23" s="17"/>
+      <c r="M23" s="17"/>
+      <c r="N23" s="17"/>
+      <c r="O23" s="17"/>
+      <c r="P23" s="17"/>
+      <c r="Q23" s="17"/>
+      <c r="R23" s="17"/>
+      <c r="S23" s="18"/>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A24" s="24"/>
-      <c r="B24" s="25"/>
-      <c r="C24" s="25"/>
-      <c r="D24" s="25"/>
-      <c r="E24" s="25"/>
-      <c r="F24" s="25"/>
-      <c r="G24" s="25"/>
-      <c r="H24" s="25"/>
-      <c r="I24" s="25"/>
-      <c r="J24" s="25"/>
-      <c r="K24" s="25"/>
-      <c r="L24" s="25"/>
-      <c r="M24" s="25"/>
-      <c r="N24" s="25"/>
-      <c r="O24" s="25"/>
-      <c r="P24" s="25"/>
-      <c r="Q24" s="25"/>
-      <c r="R24" s="25"/>
-      <c r="S24" s="26"/>
+      <c r="A24" s="16"/>
+      <c r="B24" s="17"/>
+      <c r="C24" s="17"/>
+      <c r="D24" s="17"/>
+      <c r="E24" s="17"/>
+      <c r="F24" s="17"/>
+      <c r="G24" s="17"/>
+      <c r="H24" s="17"/>
+      <c r="I24" s="17"/>
+      <c r="J24" s="17"/>
+      <c r="K24" s="17"/>
+      <c r="L24" s="17"/>
+      <c r="M24" s="17"/>
+      <c r="N24" s="17"/>
+      <c r="O24" s="17"/>
+      <c r="P24" s="17"/>
+      <c r="Q24" s="17"/>
+      <c r="R24" s="17"/>
+      <c r="S24" s="18"/>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A25" s="24"/>
-      <c r="B25" s="25"/>
-      <c r="C25" s="25"/>
-      <c r="D25" s="25"/>
-      <c r="E25" s="25"/>
-      <c r="F25" s="25"/>
-      <c r="G25" s="25"/>
-      <c r="H25" s="25"/>
-      <c r="I25" s="25"/>
-      <c r="J25" s="25"/>
-      <c r="K25" s="25"/>
-      <c r="L25" s="25"/>
-      <c r="M25" s="25"/>
-      <c r="N25" s="25"/>
-      <c r="O25" s="25"/>
-      <c r="P25" s="25"/>
-      <c r="Q25" s="25"/>
-      <c r="R25" s="25"/>
-      <c r="S25" s="26"/>
+      <c r="A25" s="16"/>
+      <c r="B25" s="17"/>
+      <c r="C25" s="17"/>
+      <c r="D25" s="17"/>
+      <c r="E25" s="17"/>
+      <c r="F25" s="17"/>
+      <c r="G25" s="17"/>
+      <c r="H25" s="17"/>
+      <c r="I25" s="17"/>
+      <c r="J25" s="17"/>
+      <c r="K25" s="17"/>
+      <c r="L25" s="17"/>
+      <c r="M25" s="17"/>
+      <c r="N25" s="17"/>
+      <c r="O25" s="17"/>
+      <c r="P25" s="17"/>
+      <c r="Q25" s="17"/>
+      <c r="R25" s="17"/>
+      <c r="S25" s="18"/>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A26" s="24"/>
-      <c r="B26" s="25"/>
-      <c r="C26" s="25"/>
-      <c r="D26" s="25"/>
-      <c r="E26" s="25"/>
-      <c r="F26" s="25"/>
-      <c r="G26" s="25"/>
-      <c r="H26" s="25"/>
-      <c r="I26" s="25"/>
-      <c r="J26" s="25"/>
-      <c r="K26" s="25"/>
-      <c r="L26" s="25"/>
-      <c r="M26" s="25"/>
-      <c r="N26" s="25"/>
-      <c r="O26" s="25"/>
-      <c r="P26" s="25"/>
-      <c r="Q26" s="25"/>
-      <c r="R26" s="25"/>
-      <c r="S26" s="26"/>
+      <c r="A26" s="16"/>
+      <c r="B26" s="17"/>
+      <c r="C26" s="17"/>
+      <c r="D26" s="17"/>
+      <c r="E26" s="17"/>
+      <c r="F26" s="17"/>
+      <c r="G26" s="17"/>
+      <c r="H26" s="17"/>
+      <c r="I26" s="17"/>
+      <c r="J26" s="17"/>
+      <c r="K26" s="17"/>
+      <c r="L26" s="17"/>
+      <c r="M26" s="17"/>
+      <c r="N26" s="17"/>
+      <c r="O26" s="17"/>
+      <c r="P26" s="17"/>
+      <c r="Q26" s="17"/>
+      <c r="R26" s="17"/>
+      <c r="S26" s="18"/>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A27" s="24"/>
-      <c r="B27" s="25"/>
-      <c r="C27" s="25"/>
-      <c r="D27" s="25"/>
-      <c r="E27" s="25"/>
-      <c r="F27" s="25"/>
-      <c r="G27" s="25"/>
-      <c r="H27" s="25"/>
-      <c r="I27" s="25"/>
-      <c r="J27" s="25"/>
-      <c r="K27" s="25"/>
-      <c r="L27" s="25"/>
-      <c r="M27" s="25"/>
-      <c r="N27" s="25"/>
-      <c r="O27" s="25"/>
-      <c r="P27" s="25"/>
-      <c r="Q27" s="25"/>
-      <c r="R27" s="25"/>
-      <c r="S27" s="26"/>
+      <c r="A27" s="16"/>
+      <c r="B27" s="17"/>
+      <c r="C27" s="17"/>
+      <c r="D27" s="17"/>
+      <c r="E27" s="17"/>
+      <c r="F27" s="17"/>
+      <c r="G27" s="17"/>
+      <c r="H27" s="17"/>
+      <c r="I27" s="17"/>
+      <c r="J27" s="17"/>
+      <c r="K27" s="17"/>
+      <c r="L27" s="17"/>
+      <c r="M27" s="17"/>
+      <c r="N27" s="17"/>
+      <c r="O27" s="17"/>
+      <c r="P27" s="17"/>
+      <c r="Q27" s="17"/>
+      <c r="R27" s="17"/>
+      <c r="S27" s="18"/>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A28" s="27"/>
-      <c r="B28" s="28"/>
-      <c r="C28" s="28"/>
-      <c r="D28" s="28"/>
-      <c r="E28" s="28"/>
-      <c r="F28" s="28"/>
-      <c r="G28" s="28"/>
-      <c r="H28" s="28"/>
-      <c r="I28" s="28"/>
-      <c r="J28" s="28"/>
-      <c r="K28" s="28"/>
-      <c r="L28" s="28"/>
-      <c r="M28" s="28"/>
-      <c r="N28" s="28"/>
-      <c r="O28" s="28"/>
-      <c r="P28" s="28"/>
-      <c r="Q28" s="28"/>
-      <c r="R28" s="28"/>
-      <c r="S28" s="29"/>
+      <c r="A28" s="16"/>
+      <c r="B28" s="17"/>
+      <c r="C28" s="17"/>
+      <c r="D28" s="17"/>
+      <c r="E28" s="17"/>
+      <c r="F28" s="17"/>
+      <c r="G28" s="17"/>
+      <c r="H28" s="17"/>
+      <c r="I28" s="17"/>
+      <c r="J28" s="17"/>
+      <c r="K28" s="17"/>
+      <c r="L28" s="17"/>
+      <c r="M28" s="17"/>
+      <c r="N28" s="17"/>
+      <c r="O28" s="17"/>
+      <c r="P28" s="17"/>
+      <c r="Q28" s="17"/>
+      <c r="R28" s="17"/>
+      <c r="S28" s="18"/>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="A29" s="16"/>
+      <c r="B29" s="17"/>
+      <c r="C29" s="17"/>
+      <c r="D29" s="17"/>
+      <c r="E29" s="17"/>
+      <c r="F29" s="17"/>
+      <c r="G29" s="17"/>
+      <c r="H29" s="17"/>
+      <c r="I29" s="17"/>
+      <c r="J29" s="17"/>
+      <c r="K29" s="17"/>
+      <c r="L29" s="17"/>
+      <c r="M29" s="17"/>
+      <c r="N29" s="17"/>
+      <c r="O29" s="17"/>
+      <c r="P29" s="17"/>
+      <c r="Q29" s="17"/>
+      <c r="R29" s="17"/>
+      <c r="S29" s="18"/>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="A30" s="16"/>
+      <c r="B30" s="35" t="s">
+        <v>68</v>
+      </c>
+      <c r="C30" s="35"/>
+      <c r="D30" s="35"/>
+      <c r="E30" s="17"/>
+      <c r="F30" s="17"/>
+      <c r="G30" s="17"/>
+      <c r="H30" s="17"/>
+      <c r="I30" s="17"/>
+      <c r="J30" s="17"/>
+      <c r="K30" s="17"/>
+      <c r="L30" s="17"/>
+      <c r="M30" s="17"/>
+      <c r="N30" s="17"/>
+      <c r="O30" s="17"/>
+      <c r="P30" s="17"/>
+      <c r="Q30" s="17"/>
+      <c r="R30" s="17"/>
+      <c r="S30" s="18"/>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="A31" s="16"/>
+      <c r="B31" s="17"/>
+      <c r="C31" s="17"/>
+      <c r="D31" s="17"/>
+      <c r="E31" s="17"/>
+      <c r="F31" s="17"/>
+      <c r="G31" s="17"/>
+      <c r="H31" s="17"/>
+      <c r="I31" s="17"/>
+      <c r="J31" s="17"/>
+      <c r="K31" s="17"/>
+      <c r="L31" s="17"/>
+      <c r="M31" s="17"/>
+      <c r="N31" s="17"/>
+      <c r="O31" s="17"/>
+      <c r="P31" s="17"/>
+      <c r="Q31" s="17"/>
+      <c r="R31" s="17"/>
+      <c r="S31" s="18"/>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="A32" s="16"/>
+      <c r="B32" s="17"/>
+      <c r="C32" s="17"/>
+      <c r="D32" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="E32" s="17"/>
+      <c r="F32" s="17"/>
+      <c r="G32" s="17"/>
+      <c r="H32" s="17"/>
+      <c r="I32" s="17"/>
+      <c r="J32" s="17"/>
+      <c r="K32" s="17"/>
+      <c r="L32" s="17"/>
+      <c r="M32" s="17"/>
+      <c r="N32" s="17"/>
+      <c r="O32" s="17"/>
+      <c r="P32" s="17"/>
+      <c r="Q32" s="17"/>
+      <c r="R32" s="17"/>
+      <c r="S32" s="18"/>
+    </row>
+    <row r="33" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="A33" s="16"/>
+      <c r="B33" s="17"/>
+      <c r="C33" s="17"/>
+      <c r="D33" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="E33" s="17"/>
+      <c r="F33" s="17"/>
+      <c r="G33" s="17"/>
+      <c r="H33" s="17"/>
+      <c r="I33" s="17"/>
+      <c r="J33" s="17"/>
+      <c r="K33" s="17"/>
+      <c r="L33" s="17"/>
+      <c r="M33" s="17"/>
+      <c r="N33" s="17"/>
+      <c r="O33" s="17"/>
+      <c r="P33" s="17"/>
+      <c r="Q33" s="17"/>
+      <c r="R33" s="17"/>
+      <c r="S33" s="18"/>
+    </row>
+    <row r="34" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="A34" s="16"/>
+      <c r="B34" s="17"/>
+      <c r="C34" s="17"/>
+      <c r="D34" s="17"/>
+      <c r="E34" s="17"/>
+      <c r="F34" s="17"/>
+      <c r="G34" s="17"/>
+      <c r="H34" s="17"/>
+      <c r="I34" s="17"/>
+      <c r="J34" s="17"/>
+      <c r="K34" s="17"/>
+      <c r="L34" s="17"/>
+      <c r="M34" s="17"/>
+      <c r="N34" s="17"/>
+      <c r="O34" s="17"/>
+      <c r="P34" s="17"/>
+      <c r="Q34" s="17"/>
+      <c r="R34" s="17"/>
+      <c r="S34" s="18"/>
+    </row>
+    <row r="35" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="A35" s="16"/>
+      <c r="B35" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="C35" s="17"/>
+      <c r="D35" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="E35" s="17"/>
+      <c r="F35" s="17"/>
+      <c r="G35" s="17"/>
+      <c r="H35" s="17"/>
+      <c r="I35" s="17"/>
+      <c r="J35" s="17"/>
+      <c r="K35" s="17"/>
+      <c r="L35" s="17"/>
+      <c r="M35" s="17"/>
+      <c r="N35" s="17"/>
+      <c r="O35" s="17"/>
+      <c r="P35" s="17"/>
+      <c r="Q35" s="17"/>
+      <c r="R35" s="17"/>
+      <c r="S35" s="18"/>
+    </row>
+    <row r="36" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="A36" s="16"/>
+      <c r="B36" s="17"/>
+      <c r="C36" s="17"/>
+      <c r="D36" s="17"/>
+      <c r="E36" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="F36" s="17"/>
+      <c r="G36" s="17"/>
+      <c r="H36" s="17"/>
+      <c r="I36" s="17"/>
+      <c r="J36" s="17"/>
+      <c r="K36" s="17"/>
+      <c r="L36" s="17"/>
+      <c r="M36" s="17"/>
+      <c r="N36" s="17"/>
+      <c r="O36" s="17"/>
+      <c r="P36" s="17"/>
+      <c r="Q36" s="17"/>
+      <c r="R36" s="17"/>
+      <c r="S36" s="18"/>
+    </row>
+    <row r="37" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="A37" s="16"/>
+      <c r="B37" s="17"/>
+      <c r="C37" s="17"/>
+      <c r="D37" s="17"/>
+      <c r="E37" s="17"/>
+      <c r="F37" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="G37" s="17"/>
+      <c r="H37" s="17"/>
+      <c r="I37" s="17"/>
+      <c r="J37" s="17"/>
+      <c r="K37" s="17"/>
+      <c r="L37" s="17"/>
+      <c r="M37" s="17"/>
+      <c r="N37" s="17"/>
+      <c r="O37" s="17"/>
+      <c r="P37" s="17"/>
+      <c r="Q37" s="17"/>
+      <c r="R37" s="17"/>
+      <c r="S37" s="18"/>
+    </row>
+    <row r="38" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="A38" s="16"/>
+      <c r="B38" s="17"/>
+      <c r="C38" s="17"/>
+      <c r="D38" s="17"/>
+      <c r="E38" s="17"/>
+      <c r="F38" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="G38" s="17"/>
+      <c r="H38" s="17"/>
+      <c r="I38" s="17"/>
+      <c r="J38" s="17"/>
+      <c r="K38" s="17"/>
+      <c r="L38" s="17"/>
+      <c r="M38" s="17"/>
+      <c r="N38" s="17"/>
+      <c r="O38" s="17"/>
+      <c r="P38" s="17"/>
+      <c r="Q38" s="17"/>
+      <c r="R38" s="17"/>
+      <c r="S38" s="18"/>
+    </row>
+    <row r="39" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="A39" s="16"/>
+      <c r="B39" s="17"/>
+      <c r="C39" s="17"/>
+      <c r="D39" s="17"/>
+      <c r="E39" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="F39" s="17"/>
+      <c r="G39" s="17"/>
+      <c r="H39" s="17"/>
+      <c r="I39" s="17"/>
+      <c r="J39" s="36"/>
+      <c r="K39" s="36"/>
+      <c r="L39" s="36"/>
+      <c r="M39" s="36"/>
+      <c r="N39" s="36"/>
+      <c r="O39" s="36"/>
+      <c r="P39" s="17"/>
+      <c r="Q39" s="17"/>
+      <c r="R39" s="17"/>
+      <c r="S39" s="18"/>
+    </row>
+    <row r="40" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="A40" s="16"/>
+      <c r="B40" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="C40" s="17"/>
+      <c r="D40" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="E40" s="17"/>
+      <c r="F40" s="17"/>
+      <c r="G40" s="17"/>
+      <c r="H40" s="17"/>
+      <c r="I40" s="17"/>
+      <c r="J40" s="17"/>
+      <c r="K40" s="17"/>
+      <c r="L40" s="17"/>
+      <c r="M40" s="17"/>
+      <c r="N40" s="17"/>
+      <c r="O40" s="17"/>
+      <c r="P40" s="17"/>
+      <c r="Q40" s="17"/>
+      <c r="R40" s="17"/>
+      <c r="S40" s="18"/>
+    </row>
+    <row r="41" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="A41" s="16"/>
+      <c r="B41" s="17"/>
+      <c r="C41" s="17"/>
+      <c r="D41" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="E41" s="17"/>
+      <c r="F41" s="17"/>
+      <c r="G41" s="17"/>
+      <c r="H41" s="17"/>
+      <c r="I41" s="17"/>
+      <c r="J41" s="17"/>
+      <c r="K41" s="17"/>
+      <c r="L41" s="17"/>
+      <c r="M41" s="17"/>
+      <c r="N41" s="17"/>
+      <c r="O41" s="17"/>
+      <c r="P41" s="17"/>
+      <c r="Q41" s="17"/>
+      <c r="R41" s="17"/>
+      <c r="S41" s="18"/>
+    </row>
+    <row r="42" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="A42" s="19"/>
+      <c r="B42" s="20"/>
+      <c r="C42" s="20"/>
+      <c r="D42" s="20"/>
+      <c r="E42" s="20"/>
+      <c r="F42" s="20"/>
+      <c r="G42" s="20"/>
+      <c r="H42" s="20"/>
+      <c r="I42" s="20"/>
+      <c r="J42" s="20"/>
+      <c r="K42" s="20"/>
+      <c r="L42" s="20"/>
+      <c r="M42" s="20"/>
+      <c r="N42" s="20"/>
+      <c r="O42" s="20"/>
+      <c r="P42" s="20"/>
+      <c r="Q42" s="20"/>
+      <c r="R42" s="20"/>
+      <c r="S42" s="21"/>
+    </row>
+    <row r="44" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="A44" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="B44" s="14"/>
+      <c r="C44" s="14"/>
+      <c r="D44" s="14"/>
+      <c r="E44" s="14"/>
+      <c r="F44" s="14"/>
+      <c r="G44" s="14"/>
+      <c r="H44" s="14"/>
+      <c r="I44" s="14"/>
+      <c r="J44" s="14"/>
+      <c r="K44" s="14"/>
+      <c r="L44" s="14"/>
+      <c r="M44" s="14"/>
+      <c r="N44" s="14"/>
+      <c r="O44" s="14"/>
+      <c r="P44" s="14"/>
+      <c r="Q44" s="14"/>
+      <c r="R44" s="14"/>
+      <c r="S44" s="14"/>
+      <c r="T44" s="14"/>
+      <c r="U44" s="14"/>
+      <c r="V44" s="14"/>
+      <c r="W44" s="15"/>
+    </row>
+    <row r="45" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A45" s="38"/>
+      <c r="B45" s="39" t="s">
+        <v>101</v>
+      </c>
+      <c r="C45" s="39"/>
+      <c r="D45" s="17"/>
+      <c r="E45" s="17"/>
+      <c r="F45" s="17"/>
+      <c r="G45" s="17"/>
+      <c r="H45" s="17"/>
+      <c r="I45" s="17"/>
+      <c r="J45" s="17"/>
+      <c r="K45" s="17"/>
+      <c r="L45" s="17"/>
+      <c r="M45" s="17"/>
+      <c r="N45" s="17"/>
+      <c r="O45" s="17"/>
+      <c r="P45" s="17"/>
+      <c r="Q45" s="17"/>
+      <c r="R45" s="17"/>
+      <c r="S45" s="17"/>
+      <c r="T45" s="17"/>
+      <c r="U45" s="17"/>
+      <c r="V45" s="17"/>
+      <c r="W45" s="18"/>
+    </row>
+    <row r="46" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="A46" s="16"/>
+      <c r="B46" s="17"/>
+      <c r="C46" s="17"/>
+      <c r="D46" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="E46" s="17"/>
+      <c r="F46" s="17"/>
+      <c r="G46" s="17"/>
+      <c r="H46" s="17"/>
+      <c r="I46" s="17"/>
+      <c r="J46" s="17"/>
+      <c r="K46" s="17"/>
+      <c r="L46" s="17"/>
+      <c r="M46" s="17"/>
+      <c r="N46" s="17"/>
+      <c r="O46" s="17"/>
+      <c r="P46" s="17"/>
+      <c r="Q46" s="17"/>
+      <c r="R46" s="17"/>
+      <c r="S46" s="17"/>
+      <c r="T46" s="17"/>
+      <c r="U46" s="17"/>
+      <c r="V46" s="17"/>
+      <c r="W46" s="18"/>
+    </row>
+    <row r="47" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="A47" s="16"/>
+      <c r="B47" s="17"/>
+      <c r="C47" s="17"/>
+      <c r="D47" s="17"/>
+      <c r="E47" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="F47" s="17"/>
+      <c r="G47" s="17"/>
+      <c r="H47" s="17"/>
+      <c r="I47" s="17"/>
+      <c r="J47" s="17"/>
+      <c r="K47" s="17"/>
+      <c r="L47" s="17"/>
+      <c r="M47" s="17"/>
+      <c r="N47" s="17"/>
+      <c r="O47" s="17"/>
+      <c r="P47" s="17"/>
+      <c r="Q47" s="17"/>
+      <c r="R47" s="17"/>
+      <c r="S47" s="17"/>
+      <c r="T47" s="17"/>
+      <c r="U47" s="17"/>
+      <c r="V47" s="17"/>
+      <c r="W47" s="18"/>
+    </row>
+    <row r="48" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="A48" s="16"/>
+      <c r="B48" s="17"/>
+      <c r="C48" s="17"/>
+      <c r="D48" s="17"/>
+      <c r="E48" s="17"/>
+      <c r="F48" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="G48" s="17"/>
+      <c r="H48" s="17"/>
+      <c r="I48" s="17"/>
+      <c r="J48" s="17"/>
+      <c r="K48" s="17"/>
+      <c r="L48" s="17"/>
+      <c r="M48" s="17"/>
+      <c r="N48" s="17"/>
+      <c r="O48" s="17"/>
+      <c r="P48" s="17"/>
+      <c r="Q48" s="17"/>
+      <c r="R48" s="17"/>
+      <c r="S48" s="17"/>
+      <c r="T48" s="17"/>
+      <c r="U48" s="17"/>
+      <c r="V48" s="17"/>
+      <c r="W48" s="18"/>
+    </row>
+    <row r="49" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="A49" s="16"/>
+      <c r="B49" s="17"/>
+      <c r="C49" s="17"/>
+      <c r="D49" s="17"/>
+      <c r="E49" s="17"/>
+      <c r="F49" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="G49" s="17"/>
+      <c r="H49" s="17"/>
+      <c r="I49" s="17"/>
+      <c r="J49" s="17"/>
+      <c r="K49" s="17"/>
+      <c r="L49" s="17"/>
+      <c r="M49" s="17"/>
+      <c r="N49" s="17"/>
+      <c r="O49" s="17"/>
+      <c r="P49" s="17"/>
+      <c r="Q49" s="17"/>
+      <c r="R49" s="17"/>
+      <c r="S49" s="17"/>
+      <c r="T49" s="17"/>
+      <c r="U49" s="17"/>
+      <c r="V49" s="17"/>
+      <c r="W49" s="18"/>
+    </row>
+    <row r="50" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="A50" s="16"/>
+      <c r="B50" s="17"/>
+      <c r="C50" s="17"/>
+      <c r="D50" s="17"/>
+      <c r="E50" s="17"/>
+      <c r="F50" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="G50" s="17"/>
+      <c r="H50" s="17"/>
+      <c r="I50" s="17"/>
+      <c r="J50" s="17"/>
+      <c r="K50" s="17"/>
+      <c r="L50" s="17"/>
+      <c r="M50" s="17"/>
+      <c r="N50" s="17"/>
+      <c r="O50" s="17"/>
+      <c r="P50" s="17"/>
+      <c r="Q50" s="17"/>
+      <c r="R50" s="17"/>
+      <c r="S50" s="17"/>
+      <c r="T50" s="17"/>
+      <c r="U50" s="17"/>
+      <c r="V50" s="17"/>
+      <c r="W50" s="18"/>
+    </row>
+    <row r="51" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="A51" s="16"/>
+      <c r="B51" s="17"/>
+      <c r="C51" s="17"/>
+      <c r="D51" s="17"/>
+      <c r="E51" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="F51" s="17"/>
+      <c r="G51" s="17"/>
+      <c r="H51" s="17"/>
+      <c r="I51" s="17"/>
+      <c r="J51" s="17"/>
+      <c r="K51" s="17"/>
+      <c r="L51" s="17"/>
+      <c r="M51" s="17"/>
+      <c r="N51" s="17"/>
+      <c r="O51" s="17"/>
+      <c r="P51" s="17"/>
+      <c r="Q51" s="17"/>
+      <c r="R51" s="17"/>
+      <c r="S51" s="17"/>
+      <c r="T51" s="17"/>
+      <c r="U51" s="17"/>
+      <c r="V51" s="17"/>
+      <c r="W51" s="18"/>
+    </row>
+    <row r="52" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="A52" s="16"/>
+      <c r="B52" s="17"/>
+      <c r="C52" s="17"/>
+      <c r="D52" s="17"/>
+      <c r="E52" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="F52" s="17"/>
+      <c r="G52" s="17"/>
+      <c r="H52" s="17"/>
+      <c r="I52" s="17"/>
+      <c r="J52" s="17"/>
+      <c r="K52" s="17"/>
+      <c r="L52" s="17"/>
+      <c r="M52" s="17"/>
+      <c r="N52" s="17"/>
+      <c r="O52" s="17"/>
+      <c r="P52" s="17"/>
+      <c r="Q52" s="17"/>
+      <c r="R52" s="17"/>
+      <c r="S52" s="17"/>
+      <c r="T52" s="17"/>
+      <c r="U52" s="17"/>
+      <c r="V52" s="17"/>
+      <c r="W52" s="18"/>
+    </row>
+    <row r="53" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="A53" s="16"/>
+      <c r="B53" s="17"/>
+      <c r="C53" s="17"/>
+      <c r="D53" s="17"/>
+      <c r="E53" s="17"/>
+      <c r="F53" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="G53" s="17"/>
+      <c r="H53" s="17"/>
+      <c r="I53" s="17"/>
+      <c r="J53" s="17"/>
+      <c r="K53" s="17"/>
+      <c r="L53" s="17"/>
+      <c r="M53" s="17"/>
+      <c r="N53" s="17"/>
+      <c r="O53" s="17"/>
+      <c r="P53" s="17"/>
+      <c r="Q53" s="17"/>
+      <c r="R53" s="17"/>
+      <c r="S53" s="17"/>
+      <c r="T53" s="17"/>
+      <c r="U53" s="17"/>
+      <c r="V53" s="17"/>
+      <c r="W53" s="18"/>
+    </row>
+    <row r="54" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="A54" s="16"/>
+      <c r="B54" s="17"/>
+      <c r="C54" s="17"/>
+      <c r="D54" s="17"/>
+      <c r="E54" s="17"/>
+      <c r="F54" s="17"/>
+      <c r="G54" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="H54" s="17"/>
+      <c r="I54" s="17"/>
+      <c r="J54" s="17"/>
+      <c r="K54" s="17"/>
+      <c r="L54" s="17"/>
+      <c r="M54" s="17"/>
+      <c r="N54" s="17"/>
+      <c r="O54" s="17"/>
+      <c r="P54" s="17"/>
+      <c r="Q54" s="17"/>
+      <c r="R54" s="17"/>
+      <c r="S54" s="17"/>
+      <c r="T54" s="17"/>
+      <c r="U54" s="17"/>
+      <c r="V54" s="17"/>
+      <c r="W54" s="18"/>
+    </row>
+    <row r="55" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="A55" s="16"/>
+      <c r="B55" s="17"/>
+      <c r="C55" s="17"/>
+      <c r="D55" s="17"/>
+      <c r="E55" s="17"/>
+      <c r="F55" s="17"/>
+      <c r="G55" s="40" t="s">
+        <v>85</v>
+      </c>
+      <c r="H55" s="40"/>
+      <c r="I55" s="40"/>
+      <c r="J55" s="40"/>
+      <c r="K55" s="40"/>
+      <c r="L55" s="17"/>
+      <c r="M55" s="17"/>
+      <c r="N55" s="17"/>
+      <c r="O55" s="17"/>
+      <c r="P55" s="17"/>
+      <c r="Q55" s="17"/>
+      <c r="R55" s="17"/>
+      <c r="S55" s="17"/>
+      <c r="T55" s="17"/>
+      <c r="U55" s="17"/>
+      <c r="V55" s="17"/>
+      <c r="W55" s="18"/>
+    </row>
+    <row r="56" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="A56" s="16"/>
+      <c r="B56" s="17"/>
+      <c r="C56" s="17"/>
+      <c r="D56" s="17"/>
+      <c r="E56" s="17"/>
+      <c r="F56" s="17"/>
+      <c r="G56" s="17"/>
+      <c r="H56" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="I56" s="17"/>
+      <c r="J56" s="17"/>
+      <c r="K56" s="17"/>
+      <c r="L56" s="17"/>
+      <c r="M56" s="17"/>
+      <c r="N56" s="17"/>
+      <c r="O56" s="17"/>
+      <c r="P56" s="17"/>
+      <c r="Q56" s="17"/>
+      <c r="R56" s="17"/>
+      <c r="S56" s="17"/>
+      <c r="T56" s="17"/>
+      <c r="U56" s="17"/>
+      <c r="V56" s="17"/>
+      <c r="W56" s="18"/>
+    </row>
+    <row r="57" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="A57" s="16"/>
+      <c r="B57" s="17"/>
+      <c r="C57" s="17"/>
+      <c r="D57" s="17"/>
+      <c r="E57" s="17"/>
+      <c r="F57" s="17"/>
+      <c r="G57" s="17"/>
+      <c r="H57" s="17"/>
+      <c r="I57" s="36" t="s">
+        <v>87</v>
+      </c>
+      <c r="J57" s="36"/>
+      <c r="K57" s="36"/>
+      <c r="L57" s="36"/>
+      <c r="M57" s="36"/>
+      <c r="N57" s="36"/>
+      <c r="O57" s="36"/>
+      <c r="P57" s="17"/>
+      <c r="Q57" s="17"/>
+      <c r="R57" s="17"/>
+      <c r="S57" s="17"/>
+      <c r="T57" s="17"/>
+      <c r="U57" s="17"/>
+      <c r="V57" s="17"/>
+      <c r="W57" s="18"/>
+    </row>
+    <row r="58" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="A58" s="16"/>
+      <c r="B58" s="17"/>
+      <c r="C58" s="17"/>
+      <c r="D58" s="17"/>
+      <c r="E58" s="17"/>
+      <c r="F58" s="17"/>
+      <c r="G58" s="17"/>
+      <c r="H58" s="17"/>
+      <c r="I58" s="17"/>
+      <c r="J58" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="K58" s="17"/>
+      <c r="L58" s="17"/>
+      <c r="M58" s="17"/>
+      <c r="N58" s="17"/>
+      <c r="O58" s="17"/>
+      <c r="P58" s="17"/>
+      <c r="Q58" s="17"/>
+      <c r="R58" s="17"/>
+      <c r="S58" s="17"/>
+      <c r="T58" s="17"/>
+      <c r="U58" s="17"/>
+      <c r="V58" s="17"/>
+      <c r="W58" s="18"/>
+    </row>
+    <row r="59" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="A59" s="16"/>
+      <c r="B59" s="17"/>
+      <c r="C59" s="17"/>
+      <c r="D59" s="17"/>
+      <c r="E59" s="17"/>
+      <c r="F59" s="17"/>
+      <c r="G59" s="17"/>
+      <c r="H59" s="17"/>
+      <c r="I59" s="17"/>
+      <c r="J59" s="17"/>
+      <c r="K59" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="L59" s="17"/>
+      <c r="M59" s="17"/>
+      <c r="N59" s="17"/>
+      <c r="O59" s="17"/>
+      <c r="P59" s="17"/>
+      <c r="Q59" s="17"/>
+      <c r="R59" s="17"/>
+      <c r="S59" s="17"/>
+      <c r="T59" s="17"/>
+      <c r="U59" s="17"/>
+      <c r="V59" s="17"/>
+      <c r="W59" s="18"/>
+    </row>
+    <row r="60" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="A60" s="16"/>
+      <c r="B60" s="17"/>
+      <c r="C60" s="17"/>
+      <c r="D60" s="17"/>
+      <c r="E60" s="17"/>
+      <c r="F60" s="17"/>
+      <c r="G60" s="17"/>
+      <c r="H60" s="17"/>
+      <c r="I60" s="17"/>
+      <c r="J60" s="17"/>
+      <c r="K60" s="17"/>
+      <c r="L60" s="41" t="s">
+        <v>89</v>
+      </c>
+      <c r="M60" s="41"/>
+      <c r="N60" s="41"/>
+      <c r="O60" s="41"/>
+      <c r="P60" s="41"/>
+      <c r="Q60" s="41"/>
+      <c r="R60" s="41"/>
+      <c r="S60" s="41"/>
+      <c r="T60" s="41"/>
+      <c r="U60" s="41"/>
+      <c r="V60" s="17"/>
+      <c r="W60" s="18"/>
+    </row>
+    <row r="61" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="A61" s="16"/>
+      <c r="B61" s="17"/>
+      <c r="C61" s="17"/>
+      <c r="D61" s="17"/>
+      <c r="E61" s="17"/>
+      <c r="F61" s="17"/>
+      <c r="G61" s="17"/>
+      <c r="H61" s="17"/>
+      <c r="I61" s="17"/>
+      <c r="J61" s="17"/>
+      <c r="K61" s="17"/>
+      <c r="L61" s="41"/>
+      <c r="M61" s="41" t="s">
+        <v>90</v>
+      </c>
+      <c r="N61" s="41"/>
+      <c r="O61" s="41"/>
+      <c r="P61" s="41"/>
+      <c r="Q61" s="41"/>
+      <c r="R61" s="41"/>
+      <c r="S61" s="41"/>
+      <c r="T61" s="41"/>
+      <c r="U61" s="41"/>
+      <c r="V61" s="17"/>
+      <c r="W61" s="18"/>
+    </row>
+    <row r="62" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="A62" s="16"/>
+      <c r="B62" s="17"/>
+      <c r="C62" s="17"/>
+      <c r="D62" s="17"/>
+      <c r="E62" s="17"/>
+      <c r="F62" s="17"/>
+      <c r="G62" s="17"/>
+      <c r="H62" s="17"/>
+      <c r="I62" s="17"/>
+      <c r="J62" s="17"/>
+      <c r="K62" s="17"/>
+      <c r="L62" s="41"/>
+      <c r="M62" s="41" t="s">
+        <v>91</v>
+      </c>
+      <c r="N62" s="41"/>
+      <c r="O62" s="41"/>
+      <c r="P62" s="41"/>
+      <c r="Q62" s="41"/>
+      <c r="R62" s="41"/>
+      <c r="S62" s="41"/>
+      <c r="T62" s="41"/>
+      <c r="U62" s="41"/>
+      <c r="V62" s="17"/>
+      <c r="W62" s="18"/>
+    </row>
+    <row r="63" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="A63" s="16"/>
+      <c r="B63" s="17"/>
+      <c r="C63" s="17"/>
+      <c r="D63" s="17"/>
+      <c r="E63" s="17"/>
+      <c r="F63" s="17"/>
+      <c r="G63" s="17"/>
+      <c r="H63" s="17"/>
+      <c r="I63" s="17"/>
+      <c r="J63" s="17"/>
+      <c r="K63" s="17"/>
+      <c r="L63" s="41" t="s">
+        <v>92</v>
+      </c>
+      <c r="M63" s="41"/>
+      <c r="N63" s="41"/>
+      <c r="O63" s="41"/>
+      <c r="P63" s="41"/>
+      <c r="Q63" s="41"/>
+      <c r="R63" s="41"/>
+      <c r="S63" s="41"/>
+      <c r="T63" s="41"/>
+      <c r="U63" s="41"/>
+      <c r="V63" s="17"/>
+      <c r="W63" s="18"/>
+    </row>
+    <row r="64" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="A64" s="16"/>
+      <c r="B64" s="17"/>
+      <c r="C64" s="17"/>
+      <c r="D64" s="17"/>
+      <c r="E64" s="17"/>
+      <c r="F64" s="17"/>
+      <c r="G64" s="17"/>
+      <c r="H64" s="17"/>
+      <c r="I64" s="17"/>
+      <c r="J64" s="17"/>
+      <c r="K64" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="L64" s="17"/>
+      <c r="M64" s="17"/>
+      <c r="N64" s="17"/>
+      <c r="O64" s="17"/>
+      <c r="P64" s="17"/>
+      <c r="Q64" s="17"/>
+      <c r="R64" s="17"/>
+      <c r="S64" s="17"/>
+      <c r="T64" s="17"/>
+      <c r="U64" s="17"/>
+      <c r="V64" s="17"/>
+      <c r="W64" s="18"/>
+    </row>
+    <row r="65" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="A65" s="16"/>
+      <c r="B65" s="17"/>
+      <c r="C65" s="17"/>
+      <c r="D65" s="17"/>
+      <c r="E65" s="17"/>
+      <c r="F65" s="17"/>
+      <c r="G65" s="17"/>
+      <c r="H65" s="17"/>
+      <c r="I65" s="17"/>
+      <c r="J65" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="K65" s="17"/>
+      <c r="L65" s="17"/>
+      <c r="M65" s="17"/>
+      <c r="N65" s="17"/>
+      <c r="O65" s="17"/>
+      <c r="P65" s="17"/>
+      <c r="Q65" s="17"/>
+      <c r="R65" s="17"/>
+      <c r="S65" s="17"/>
+      <c r="T65" s="17"/>
+      <c r="U65" s="17"/>
+      <c r="V65" s="17"/>
+      <c r="W65" s="18"/>
+    </row>
+    <row r="66" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="A66" s="16"/>
+      <c r="B66" s="17"/>
+      <c r="C66" s="17"/>
+      <c r="D66" s="17"/>
+      <c r="E66" s="17"/>
+      <c r="F66" s="17"/>
+      <c r="G66" s="17"/>
+      <c r="H66" s="17"/>
+      <c r="I66" s="17"/>
+      <c r="J66" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="K66" s="17"/>
+      <c r="L66" s="17"/>
+      <c r="M66" s="17"/>
+      <c r="N66" s="17"/>
+      <c r="O66" s="17"/>
+      <c r="P66" s="17"/>
+      <c r="Q66" s="17"/>
+      <c r="R66" s="17"/>
+      <c r="S66" s="17"/>
+      <c r="T66" s="17"/>
+      <c r="U66" s="17"/>
+      <c r="V66" s="17"/>
+      <c r="W66" s="18"/>
+    </row>
+    <row r="67" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="A67" s="16"/>
+      <c r="B67" s="17"/>
+      <c r="C67" s="17"/>
+      <c r="D67" s="17"/>
+      <c r="E67" s="17"/>
+      <c r="F67" s="17"/>
+      <c r="G67" s="17"/>
+      <c r="H67" s="17"/>
+      <c r="I67" s="17"/>
+      <c r="J67" s="17"/>
+      <c r="K67" s="42" t="s">
+        <v>96</v>
+      </c>
+      <c r="L67" s="42"/>
+      <c r="M67" s="42"/>
+      <c r="N67" s="42"/>
+      <c r="O67" s="42"/>
+      <c r="P67" s="42"/>
+      <c r="Q67" s="42"/>
+      <c r="R67" s="42"/>
+      <c r="S67" s="42"/>
+      <c r="T67" s="17"/>
+      <c r="U67" s="17"/>
+      <c r="V67" s="17"/>
+      <c r="W67" s="18"/>
+    </row>
+    <row r="68" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="A68" s="16"/>
+      <c r="B68" s="17"/>
+      <c r="C68" s="17"/>
+      <c r="D68" s="17"/>
+      <c r="E68" s="17"/>
+      <c r="F68" s="17"/>
+      <c r="G68" s="17"/>
+      <c r="H68" s="17"/>
+      <c r="I68" s="17"/>
+      <c r="J68" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="K68" s="17"/>
+      <c r="L68" s="17"/>
+      <c r="M68" s="17"/>
+      <c r="N68" s="17"/>
+      <c r="O68" s="17"/>
+      <c r="P68" s="17"/>
+      <c r="Q68" s="17"/>
+      <c r="R68" s="17"/>
+      <c r="S68" s="17"/>
+      <c r="T68" s="17"/>
+      <c r="U68" s="17"/>
+      <c r="V68" s="17"/>
+      <c r="W68" s="18"/>
+    </row>
+    <row r="69" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="A69" s="16"/>
+      <c r="B69" s="17"/>
+      <c r="C69" s="17"/>
+      <c r="D69" s="17"/>
+      <c r="E69" s="17"/>
+      <c r="F69" s="17"/>
+      <c r="G69" s="17"/>
+      <c r="H69" s="17"/>
+      <c r="I69" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="J69" s="17"/>
+      <c r="K69" s="17"/>
+      <c r="L69" s="17"/>
+      <c r="M69" s="17"/>
+      <c r="N69" s="17"/>
+      <c r="O69" s="17"/>
+      <c r="P69" s="17"/>
+      <c r="Q69" s="17"/>
+      <c r="R69" s="17"/>
+      <c r="S69" s="17"/>
+      <c r="T69" s="17"/>
+      <c r="U69" s="17"/>
+      <c r="V69" s="17"/>
+      <c r="W69" s="18"/>
+    </row>
+    <row r="70" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="A70" s="16"/>
+      <c r="B70" s="17"/>
+      <c r="C70" s="17"/>
+      <c r="D70" s="17"/>
+      <c r="E70" s="17"/>
+      <c r="F70" s="17"/>
+      <c r="G70" s="17"/>
+      <c r="H70" s="17"/>
+      <c r="I70" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="J70" s="17"/>
+      <c r="K70" s="17"/>
+      <c r="L70" s="17"/>
+      <c r="M70" s="17"/>
+      <c r="N70" s="17"/>
+      <c r="O70" s="17"/>
+      <c r="P70" s="17"/>
+      <c r="Q70" s="17"/>
+      <c r="R70" s="17"/>
+      <c r="S70" s="17"/>
+      <c r="T70" s="17"/>
+      <c r="U70" s="17"/>
+      <c r="V70" s="17"/>
+      <c r="W70" s="18"/>
+    </row>
+    <row r="71" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="A71" s="16"/>
+      <c r="B71" s="17"/>
+      <c r="C71" s="17"/>
+      <c r="D71" s="17"/>
+      <c r="E71" s="17"/>
+      <c r="F71" s="17"/>
+      <c r="G71" s="17"/>
+      <c r="H71" s="17"/>
+      <c r="I71" s="17"/>
+      <c r="J71" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="K71" s="17"/>
+      <c r="L71" s="17"/>
+      <c r="M71" s="17"/>
+      <c r="N71" s="17"/>
+      <c r="O71" s="17"/>
+      <c r="P71" s="17"/>
+      <c r="Q71" s="17"/>
+      <c r="R71" s="17"/>
+      <c r="S71" s="17"/>
+      <c r="T71" s="17"/>
+      <c r="U71" s="17"/>
+      <c r="V71" s="17"/>
+      <c r="W71" s="18"/>
+    </row>
+    <row r="72" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="A72" s="16"/>
+      <c r="B72" s="17"/>
+      <c r="C72" s="17"/>
+      <c r="D72" s="17"/>
+      <c r="E72" s="17"/>
+      <c r="F72" s="17"/>
+      <c r="G72" s="17"/>
+      <c r="H72" s="17"/>
+      <c r="I72" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="J72" s="17"/>
+      <c r="K72" s="17"/>
+      <c r="L72" s="17"/>
+      <c r="M72" s="17"/>
+      <c r="N72" s="17"/>
+      <c r="O72" s="17"/>
+      <c r="P72" s="17"/>
+      <c r="Q72" s="17"/>
+      <c r="R72" s="17"/>
+      <c r="S72" s="17"/>
+      <c r="T72" s="17"/>
+      <c r="U72" s="17"/>
+      <c r="V72" s="17"/>
+      <c r="W72" s="18"/>
+    </row>
+    <row r="73" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="A73" s="16"/>
+      <c r="B73" s="17"/>
+      <c r="C73" s="17"/>
+      <c r="D73" s="17"/>
+      <c r="E73" s="17"/>
+      <c r="F73" s="17"/>
+      <c r="G73" s="17"/>
+      <c r="H73" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="I73" s="17"/>
+      <c r="J73" s="17"/>
+      <c r="K73" s="17"/>
+      <c r="L73" s="17"/>
+      <c r="M73" s="17"/>
+      <c r="N73" s="17"/>
+      <c r="O73" s="17"/>
+      <c r="P73" s="17"/>
+      <c r="Q73" s="17"/>
+      <c r="R73" s="17"/>
+      <c r="S73" s="17"/>
+      <c r="T73" s="17"/>
+      <c r="U73" s="17"/>
+      <c r="V73" s="17"/>
+      <c r="W73" s="18"/>
+    </row>
+    <row r="74" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="A74" s="16"/>
+      <c r="B74" s="17"/>
+      <c r="C74" s="17"/>
+      <c r="D74" s="17"/>
+      <c r="E74" s="17"/>
+      <c r="F74" s="17"/>
+      <c r="G74" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="H74" s="17"/>
+      <c r="I74" s="17"/>
+      <c r="J74" s="17"/>
+      <c r="K74" s="17"/>
+      <c r="L74" s="17"/>
+      <c r="M74" s="17"/>
+      <c r="N74" s="17"/>
+      <c r="O74" s="17"/>
+      <c r="P74" s="17"/>
+      <c r="Q74" s="17"/>
+      <c r="R74" s="17"/>
+      <c r="S74" s="17"/>
+      <c r="T74" s="17"/>
+      <c r="U74" s="17"/>
+      <c r="V74" s="17"/>
+      <c r="W74" s="18"/>
+    </row>
+    <row r="75" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="A75" s="16"/>
+      <c r="B75" s="17"/>
+      <c r="C75" s="17"/>
+      <c r="D75" s="17"/>
+      <c r="E75" s="17"/>
+      <c r="F75" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="G75" s="17"/>
+      <c r="H75" s="17"/>
+      <c r="I75" s="17"/>
+      <c r="J75" s="17"/>
+      <c r="K75" s="17"/>
+      <c r="L75" s="17"/>
+      <c r="M75" s="17"/>
+      <c r="N75" s="17"/>
+      <c r="O75" s="17"/>
+      <c r="P75" s="17"/>
+      <c r="Q75" s="17"/>
+      <c r="R75" s="17"/>
+      <c r="S75" s="17"/>
+      <c r="T75" s="17"/>
+      <c r="U75" s="17"/>
+      <c r="V75" s="17"/>
+      <c r="W75" s="18"/>
+    </row>
+    <row r="76" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="A76" s="16"/>
+      <c r="B76" s="17"/>
+      <c r="C76" s="17"/>
+      <c r="D76" s="17"/>
+      <c r="E76" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="F76" s="17"/>
+      <c r="G76" s="17"/>
+      <c r="H76" s="17"/>
+      <c r="I76" s="17"/>
+      <c r="J76" s="17"/>
+      <c r="K76" s="17"/>
+      <c r="L76" s="17"/>
+      <c r="M76" s="17"/>
+      <c r="N76" s="17"/>
+      <c r="O76" s="17"/>
+      <c r="P76" s="17"/>
+      <c r="Q76" s="17"/>
+      <c r="R76" s="17"/>
+      <c r="S76" s="17"/>
+      <c r="T76" s="17"/>
+      <c r="U76" s="17"/>
+      <c r="V76" s="17"/>
+      <c r="W76" s="18"/>
+    </row>
+    <row r="77" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="A77" s="16"/>
+      <c r="B77" s="17"/>
+      <c r="C77" s="17"/>
+      <c r="D77" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="E77" s="17"/>
+      <c r="F77" s="17"/>
+      <c r="G77" s="17"/>
+      <c r="H77" s="17"/>
+      <c r="I77" s="17"/>
+      <c r="J77" s="17"/>
+      <c r="K77" s="17"/>
+      <c r="L77" s="17"/>
+      <c r="M77" s="17"/>
+      <c r="N77" s="17"/>
+      <c r="O77" s="17"/>
+      <c r="P77" s="17"/>
+      <c r="Q77" s="17"/>
+      <c r="R77" s="17"/>
+      <c r="S77" s="17"/>
+      <c r="T77" s="17"/>
+      <c r="U77" s="17"/>
+      <c r="V77" s="17"/>
+      <c r="W77" s="18"/>
+    </row>
+    <row r="78" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="A78" s="16"/>
+      <c r="B78" s="17"/>
+      <c r="C78" s="17"/>
+      <c r="D78" s="17"/>
+      <c r="E78" s="17"/>
+      <c r="F78" s="17"/>
+      <c r="G78" s="17"/>
+      <c r="H78" s="17"/>
+      <c r="I78" s="17"/>
+      <c r="J78" s="17"/>
+      <c r="K78" s="17"/>
+      <c r="L78" s="17"/>
+      <c r="M78" s="17"/>
+      <c r="N78" s="17"/>
+      <c r="O78" s="17"/>
+      <c r="P78" s="17"/>
+      <c r="Q78" s="17"/>
+      <c r="R78" s="17"/>
+      <c r="S78" s="17"/>
+      <c r="T78" s="17"/>
+      <c r="U78" s="17"/>
+      <c r="V78" s="17"/>
+      <c r="W78" s="18"/>
+    </row>
+    <row r="79" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="A79" s="16"/>
+      <c r="B79" s="35" t="s">
+        <v>68</v>
+      </c>
+      <c r="C79" s="35"/>
+      <c r="D79" s="35"/>
+      <c r="E79" s="17"/>
+      <c r="F79" s="17"/>
+      <c r="G79" s="17"/>
+      <c r="H79" s="17"/>
+      <c r="I79" s="17"/>
+      <c r="J79" s="17"/>
+      <c r="K79" s="17"/>
+      <c r="L79" s="17"/>
+      <c r="M79" s="17"/>
+      <c r="N79" s="17"/>
+      <c r="O79" s="17"/>
+      <c r="P79" s="17"/>
+      <c r="Q79" s="17"/>
+      <c r="R79" s="17"/>
+      <c r="S79" s="17"/>
+      <c r="T79" s="17"/>
+      <c r="U79" s="17"/>
+      <c r="V79" s="17"/>
+      <c r="W79" s="18"/>
+    </row>
+    <row r="80" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="A80" s="19"/>
+      <c r="B80" s="20"/>
+      <c r="C80" s="20"/>
+      <c r="D80" s="20" t="s">
+        <v>102</v>
+      </c>
+      <c r="E80" s="20"/>
+      <c r="F80" s="20"/>
+      <c r="G80" s="20"/>
+      <c r="H80" s="20"/>
+      <c r="I80" s="20"/>
+      <c r="J80" s="20"/>
+      <c r="K80" s="20"/>
+      <c r="L80" s="20"/>
+      <c r="M80" s="20"/>
+      <c r="N80" s="20"/>
+      <c r="O80" s="20"/>
+      <c r="P80" s="20"/>
+      <c r="Q80" s="20"/>
+      <c r="R80" s="20"/>
+      <c r="S80" s="20"/>
+      <c r="T80" s="20"/>
+      <c r="U80" s="20"/>
+      <c r="V80" s="20"/>
+      <c r="W80" s="21"/>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B79:D79"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Dev Document UPD 20200311 Cao
</commit_message>
<xml_diff>
--- a/src/main/resources/DOC/FreeProject-Develop.xlsx
+++ b/src/main/resources/DOC/FreeProject-Develop.xlsx
@@ -1,15 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21029"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A37F51B-C910-4069-9251-871E7A99A419}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FreePj-Doc-v1" sheetId="1" r:id="rId1"/>
     <sheet name="FreePj-Develop-Ready" sheetId="2" r:id="rId2"/>
     <sheet name="Developer-Read" sheetId="3" r:id="rId3"/>
+    <sheet name="开发流程" sheetId="4" r:id="rId4"/>
+    <sheet name="共通方法" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Developer-Read'!$A$1:$B$2</definedName>
@@ -20,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="196">
   <si>
     <t>2.功能设想:</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -424,12 +427,365 @@
   <si>
     <t>private List&lt;Integer&gt; authorityId = new ArrayList&lt;Integer&gt;();</t>
   </si>
+  <si>
+    <t>freeProject\src\main\webapp\js</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>路径</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>文件名</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>方法名</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>功能</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>main.js</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>enableTooltip</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>启用提示框</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>setSearchDisabled</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>setSearchEnabled</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>禁用导航部的查询按钮</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>启用导航部的查询按钮</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>setUpdateDisabled</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>禁用导航部的更新按钮</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>setUpdateEnabled</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>setRegisteredDisabled</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>setRegisteredEnabled</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>禁用导航部的注册按钮</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>启用导航部的更新按钮</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>setActionMode</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>显示当前的画面操作</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>参数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>search</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>update</t>
+  </si>
+  <si>
+    <t>空</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>confirmTransitionHtml</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>关联</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>getSysTime</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>获取当前时间</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>docId</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>format</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>参数注释</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>元素ID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>返回时间的格式
+window.DATE_FROMAT_YYYYMMDDHHMMSS
+默认为:yyyy年MM月DD日 hh:mi:ss</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>loadDateComponent</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>时间控件</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bootstrapDateChange</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>时间控件和后台交互的问题解决</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>currentElement</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>obj</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ClearForm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>清除Form的内容</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>form的ID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1，</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DB的(t_menu)中注册开发的菜单信息【参照Sheet：FreePj-Doc-v1的规则进行开发】</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2，</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>$(function() {</t>
+  </si>
+  <si>
+    <t>// enable tooltip</t>
+  </si>
+  <si>
+    <t>enableTooltip();</t>
+  </si>
+  <si>
+    <t>// define display switch of numbers</t>
+  </si>
+  <si>
+    <t>var switchNums = 5;</t>
+  </si>
+  <si>
+    <t>// define total page numbers</t>
+  </si>
+  <si>
+    <t>var totoalPage = 20;</t>
+  </si>
+  <si>
+    <t>setSwitchBtnNums("init", switchNums, totoalPage, null, null);</t>
+  </si>
+  <si>
+    <t>/**</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> * Common: Date component</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> */</t>
+  </si>
+  <si>
+    <t>// All button enable</t>
+  </si>
+  <si>
+    <t>setSearchEnabled();</t>
+  </si>
+  <si>
+    <t>setRegisteredEnabled();</t>
+  </si>
+  <si>
+    <t>});</t>
+  </si>
+  <si>
+    <t>新建jsp(可复制sys0501.jsp),并将下面红色内容加入jsp中</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>共同方法</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>※红色内容可参考Sheet：</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>setUpdateDisabled();</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>freeProject\src\main\webapp\WEB-INF\jsp\</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>transitionHtml</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pageId</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>actionId</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>确认当前点击菜单是否要进行画面跳转</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>首次进入默认为初始化操作:当前actionId为空；点击检索等操作进入时，pageId为初始化记住的ID，actionId为当前动作标识</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>开发页面的ID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>检索等标识符(serach)，和后台的访问名一致：@RequestMapping("search")</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>menu.jsp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>freeProject\src\main\webapp\WEB-INF\jsp\template</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>setMenuContent</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>将AJAX获取的菜单信息显示到JSP上</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>msg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DB(t_menu)的信息</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>※共通方法均可以在自己的JSP中重写</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3,</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>btnName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>自定义按钮名称，可以为空</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;form role="form" id="commonForm" method="post"&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;label for="name"&gt;意见收集处&lt;/label&gt; </t>
+  </si>
+  <si>
+    <t>&lt;textarea class="form-control" rows="5" placeholder="请输入您需要解决的问题" name="opinionText"&gt;&lt;/textarea&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p class="help-block"&gt;感谢您提出的意见，我们将会对其进行分析并修正。&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;/form&gt;</t>
+  </si>
+  <si>
+    <t>5,</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>新建Controller,Service,Dao层java文件(可复制sys0501)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6，</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>新建Form,SerarchDto,ResultDto实体类(可复制sys0501)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -520,8 +876,55 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="微软雅黑"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="微软雅黑"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="微软雅黑"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="微软雅黑"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -558,8 +961,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -662,11 +1071,147 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="dotted">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="dotted">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dotted">
+        <color auto="1"/>
+      </left>
+      <right style="dotted">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="dotted">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dotted">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="dotted">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="dotted">
+        <color auto="1"/>
+      </right>
+      <top style="dotted">
+        <color auto="1"/>
+      </top>
+      <bottom style="dotted">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dotted">
+        <color auto="1"/>
+      </left>
+      <right style="dotted">
+        <color auto="1"/>
+      </right>
+      <top style="dotted">
+        <color auto="1"/>
+      </top>
+      <bottom style="dotted">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dotted">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="dotted">
+        <color auto="1"/>
+      </top>
+      <bottom style="dotted">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="dotted">
+        <color auto="1"/>
+      </right>
+      <top style="dotted">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dotted">
+        <color auto="1"/>
+      </left>
+      <right style="dotted">
+        <color auto="1"/>
+      </right>
+      <top style="dotted">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dotted">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="dotted">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -701,6 +1246,12 @@
     <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -727,24 +1278,91 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="15" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="超链接" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -767,7 +1385,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="图片 1"/>
+        <xdr:cNvPr id="2" name="图片 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -805,7 +1429,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="图片 2"/>
+        <xdr:cNvPr id="3" name="图片 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -843,7 +1473,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="矩形 3"/>
+        <xdr:cNvPr id="4" name="矩形 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -903,7 +1539,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="矩形标注 4"/>
+        <xdr:cNvPr id="5" name="矩形标注 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -971,7 +1613,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="下箭头 5"/>
+        <xdr:cNvPr id="6" name="下箭头 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1025,7 +1673,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="7" name="图片 6"/>
+        <xdr:cNvPr id="7" name="图片 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1063,7 +1717,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="8" name="矩形 7"/>
+        <xdr:cNvPr id="8" name="矩形 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000008000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1123,7 +1783,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="9" name="矩形标注 8"/>
+        <xdr:cNvPr id="9" name="矩形标注 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000009000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1220,7 +1886,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="矩形标注 1"/>
+        <xdr:cNvPr id="2" name="矩形标注 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1304,7 +1976,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="矩形标注 2"/>
+        <xdr:cNvPr id="3" name="矩形标注 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1409,7 +2087,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="矩形 3"/>
+        <xdr:cNvPr id="4" name="矩形 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1469,7 +2153,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="矩形标注 4"/>
+        <xdr:cNvPr id="5" name="矩形标注 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1541,7 +2231,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="矩形标注 5"/>
+        <xdr:cNvPr id="6" name="矩形标注 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1622,7 +2318,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="7" name="圆角矩形标注 6"/>
+        <xdr:cNvPr id="7" name="圆角矩形标注 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1683,7 +2385,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="8" name="矩形标注 7"/>
+        <xdr:cNvPr id="8" name="矩形标注 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000008000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1767,7 +2475,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="9" name="矩形标注 8"/>
+        <xdr:cNvPr id="9" name="矩形标注 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000009000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1807,6 +2521,102 @@
             <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
             <a:t>内层循环没有打印时进行本次外层循环的打印数据</a:t>
           </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>548640</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>83820</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="对话气泡: 矩形 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0E9E0B10-ECFF-4ADB-BE6D-6DA25BB2544E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4343400" y="3589020"/>
+          <a:ext cx="1691640" cy="662940"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -91554"/>
+            <a:gd name="adj2" fmla="val 40661"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
+            <a:t>form</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
+            <a:t>的</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
+            <a:t>ID</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
+            <a:t>是共通的</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
+            <a:t>commonForm</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
+            <a:t>，详情参考</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
+            <a:t>JS:transitionHtml</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -1858,7 +2668,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1891,9 +2701,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1926,6 +2753,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2101,125 +2945,125 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor rgb="FF002060"/>
   </sheetPr>
   <dimension ref="A1:P29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
-      <c r="D1" s="27" t="s">
+      <c r="D1" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
       <c r="J1" s="3"/>
       <c r="K1" s="3"/>
       <c r="L1" s="3"/>
       <c r="M1" s="3"/>
       <c r="N1" s="3"/>
-      <c r="O1" s="26" t="s">
+      <c r="O1" s="32" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="27"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="33"/>
+      <c r="I2" s="33"/>
       <c r="J2" s="3"/>
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
       <c r="N2" s="3"/>
-      <c r="O2" s="26"/>
+      <c r="O2" s="32"/>
       <c r="P2" s="7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="B3" s="30" t="s">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B3" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30"/>
-      <c r="G3" s="30"/>
-      <c r="H3" s="30"/>
-      <c r="I3" s="30"/>
-      <c r="J3" s="30"/>
-      <c r="K3" s="30"/>
-      <c r="L3" s="30"/>
-      <c r="M3" s="30"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="36"/>
+      <c r="G3" s="36"/>
+      <c r="H3" s="36"/>
+      <c r="I3" s="36"/>
+      <c r="J3" s="36"/>
+      <c r="K3" s="36"/>
+      <c r="L3" s="36"/>
+      <c r="M3" s="36"/>
       <c r="O3" s="2"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="B4" s="30"/>
-      <c r="C4" s="30"/>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="30"/>
-      <c r="G4" s="30"/>
-      <c r="H4" s="30"/>
-      <c r="I4" s="30"/>
-      <c r="J4" s="30"/>
-      <c r="K4" s="30"/>
-      <c r="L4" s="30"/>
-      <c r="M4" s="30"/>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B4" s="36"/>
+      <c r="C4" s="36"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="36"/>
+      <c r="F4" s="36"/>
+      <c r="G4" s="36"/>
+      <c r="H4" s="36"/>
+      <c r="I4" s="36"/>
+      <c r="J4" s="36"/>
+      <c r="K4" s="36"/>
+      <c r="L4" s="36"/>
+      <c r="M4" s="36"/>
       <c r="O4" s="6">
         <v>101</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="B5" s="29" t="s">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B5" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="29"/>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="C6" s="29" t="s">
+      <c r="C5" s="35"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C6" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="29"/>
-      <c r="E6" s="29"/>
-      <c r="F6" s="29"/>
-      <c r="G6" s="29"/>
-      <c r="H6" s="29"/>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="C7" s="29" t="s">
+      <c r="D6" s="35"/>
+      <c r="E6" s="35"/>
+      <c r="F6" s="35"/>
+      <c r="G6" s="35"/>
+      <c r="H6" s="35"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C7" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="29"/>
-      <c r="E7" s="29"/>
-      <c r="F7" s="29"/>
-      <c r="G7" s="29"/>
-      <c r="H7" s="29"/>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="D7" s="35"/>
+      <c r="E7" s="35"/>
+      <c r="F7" s="35"/>
+      <c r="G7" s="35"/>
+      <c r="H7" s="35"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C8" s="5">
         <v>101</v>
       </c>
@@ -2231,58 +3075,58 @@
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D9" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D10" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D13" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="D14" s="28" t="s">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="D14" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="E14" s="28"/>
-      <c r="F14" s="28"/>
-      <c r="G14" s="28"/>
-      <c r="H14" s="28"/>
-      <c r="I14" s="28"/>
-      <c r="J14" s="28"/>
-      <c r="K14" s="28"/>
-      <c r="L14" s="28"/>
-      <c r="M14" s="28"/>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="D15" s="28"/>
-      <c r="E15" s="28"/>
-      <c r="F15" s="28"/>
-      <c r="G15" s="28"/>
-      <c r="H15" s="28"/>
-      <c r="I15" s="28"/>
-      <c r="J15" s="28"/>
-      <c r="K15" s="28"/>
-      <c r="L15" s="28"/>
-      <c r="M15" s="28"/>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="E14" s="34"/>
+      <c r="F14" s="34"/>
+      <c r="G14" s="34"/>
+      <c r="H14" s="34"/>
+      <c r="I14" s="34"/>
+      <c r="J14" s="34"/>
+      <c r="K14" s="34"/>
+      <c r="L14" s="34"/>
+      <c r="M14" s="34"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="D15" s="34"/>
+      <c r="E15" s="34"/>
+      <c r="F15" s="34"/>
+      <c r="G15" s="34"/>
+      <c r="H15" s="34"/>
+      <c r="I15" s="34"/>
+      <c r="J15" s="34"/>
+      <c r="K15" s="34"/>
+      <c r="L15" s="34"/>
+      <c r="M15" s="34"/>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C18" s="24" t="s">
         <v>57</v>
       </c>
@@ -2290,7 +3134,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C19" s="25" t="s">
         <v>58</v>
       </c>
@@ -2298,7 +3142,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C20" s="25" t="s">
         <v>59</v>
       </c>
@@ -2306,7 +3150,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C21" s="25" t="s">
         <v>60</v>
       </c>
@@ -2314,12 +3158,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C24" s="24" t="s">
         <v>62</v>
       </c>
@@ -2327,7 +3171,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C25" s="25" t="s">
         <v>63</v>
       </c>
@@ -2335,7 +3179,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C26" s="25" t="s">
         <v>64</v>
       </c>
@@ -2343,7 +3187,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C27" s="25" t="s">
         <v>65</v>
       </c>
@@ -2351,7 +3195,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C28" s="25" t="s">
         <v>66</v>
       </c>
@@ -2359,7 +3203,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C29" s="25" t="s">
         <v>67</v>
       </c>
@@ -2368,7 +3212,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="C18:D18"/>
+  <autoFilter ref="C18:D18" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <mergeCells count="7">
     <mergeCell ref="O1:O2"/>
     <mergeCell ref="D1:I2"/>
@@ -2385,7 +3229,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
@@ -2395,34 +3239,34 @@
       <selection activeCell="H97" sqref="H97"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A1" s="31" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6" s="9" t="s">
         <v>15</v>
       </c>
       <c r="C6" s="9"/>
     </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A82" s="32" t="s">
+    <row r="82" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A82" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="B82" s="32"/>
-    </row>
-    <row r="83" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="B82" s="38"/>
+    </row>
+    <row r="83" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B83" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C83" s="33" t="s">
+      <c r="C83" s="39" t="s">
         <v>24</v>
       </c>
       <c r="D83" s="8" t="s">
@@ -2433,7 +3277,7 @@
       <c r="G83" s="8"/>
       <c r="H83" s="8"/>
       <c r="I83" s="8"/>
-      <c r="J83" s="33" t="s">
+      <c r="J83" s="39" t="s">
         <v>25</v>
       </c>
       <c r="K83" s="8" t="s">
@@ -2443,8 +3287,8 @@
       <c r="M83" s="8"/>
       <c r="N83" s="8"/>
     </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="C84" s="33"/>
+    <row r="84" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C84" s="39"/>
       <c r="D84" s="8" t="s">
         <v>19</v>
       </c>
@@ -2453,14 +3297,14 @@
       <c r="G84" s="8"/>
       <c r="H84" s="8"/>
       <c r="I84" s="8"/>
-      <c r="J84" s="33"/>
+      <c r="J84" s="39"/>
       <c r="K84" s="8" t="s">
         <v>19</v>
       </c>
       <c r="L84" s="8"/>
     </row>
-    <row r="85" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="C85" s="33"/>
+    <row r="85" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C85" s="39"/>
       <c r="D85" s="8"/>
       <c r="E85" s="8" t="s">
         <v>20</v>
@@ -2469,14 +3313,14 @@
       <c r="G85" s="8"/>
       <c r="H85" s="8"/>
       <c r="I85" s="8"/>
-      <c r="J85" s="33"/>
+      <c r="J85" s="39"/>
       <c r="K85" s="8"/>
       <c r="L85" s="8" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="86" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="C86" s="33"/>
+    <row r="86" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C86" s="39"/>
       <c r="D86" s="8"/>
       <c r="E86" s="8" t="s">
         <v>21</v>
@@ -2485,14 +3329,14 @@
       <c r="G86" s="8"/>
       <c r="H86" s="8"/>
       <c r="I86" s="8"/>
-      <c r="J86" s="33"/>
+      <c r="J86" s="39"/>
       <c r="K86" s="8"/>
       <c r="L86" s="8" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="87" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="C87" s="33"/>
+    <row r="87" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C87" s="39"/>
       <c r="D87" s="8"/>
       <c r="E87" s="8" t="s">
         <v>26</v>
@@ -2501,14 +3345,14 @@
       <c r="G87" s="8"/>
       <c r="H87" s="8"/>
       <c r="I87" s="8"/>
-      <c r="J87" s="33"/>
+      <c r="J87" s="39"/>
       <c r="K87" s="8"/>
       <c r="L87" s="8" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="88" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="C88" s="33"/>
+    <row r="88" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C88" s="39"/>
       <c r="D88" s="8" t="s">
         <v>23</v>
       </c>
@@ -2517,75 +3361,75 @@
       <c r="G88" s="8"/>
       <c r="H88" s="8"/>
       <c r="I88" s="8"/>
-      <c r="J88" s="33"/>
+      <c r="J88" s="39"/>
       <c r="K88" s="8" t="s">
         <v>23</v>
       </c>
       <c r="L88" s="8"/>
     </row>
-    <row r="89" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="C89" s="33"/>
+    <row r="89" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C89" s="39"/>
       <c r="D89" s="8"/>
-      <c r="J89" s="33"/>
-    </row>
-    <row r="90" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="C90" s="33"/>
-      <c r="J90" s="33"/>
-    </row>
-    <row r="91" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="C91" s="33"/>
-      <c r="J91" s="33"/>
-    </row>
-    <row r="92" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="C92" s="33"/>
-      <c r="J92" s="33"/>
-    </row>
-    <row r="93" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A93" s="34" t="s">
+      <c r="J89" s="39"/>
+    </row>
+    <row r="90" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C90" s="39"/>
+      <c r="J90" s="39"/>
+    </row>
+    <row r="91" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C91" s="39"/>
+      <c r="J91" s="39"/>
+    </row>
+    <row r="92" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C92" s="39"/>
+      <c r="J92" s="39"/>
+    </row>
+    <row r="93" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A93" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="B93" s="34"/>
-      <c r="C93" s="33"/>
+      <c r="B93" s="40"/>
+      <c r="C93" s="39"/>
       <c r="D93" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="J93" s="33"/>
+      <c r="J93" s="39"/>
       <c r="K93" s="8" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="94" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="C94" s="33"/>
+    <row r="94" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C94" s="39"/>
       <c r="D94" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="J94" s="33"/>
+      <c r="J94" s="39"/>
       <c r="K94" s="8" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="95" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="C95" s="33"/>
-      <c r="J95" s="33"/>
-    </row>
-    <row r="96" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="C96" s="33"/>
-      <c r="J96" s="33"/>
-    </row>
-    <row r="97" spans="3:10" x14ac:dyDescent="0.15">
-      <c r="C97" s="33"/>
-      <c r="J97" s="33"/>
-    </row>
-    <row r="98" spans="3:10" x14ac:dyDescent="0.15">
-      <c r="C98" s="33"/>
-      <c r="J98" s="33"/>
-    </row>
-    <row r="99" spans="3:10" x14ac:dyDescent="0.15">
-      <c r="C99" s="33"/>
-      <c r="J99" s="33"/>
-    </row>
-    <row r="100" spans="3:10" x14ac:dyDescent="0.15">
-      <c r="J100" s="33"/>
+    <row r="95" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C95" s="39"/>
+      <c r="J95" s="39"/>
+    </row>
+    <row r="96" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C96" s="39"/>
+      <c r="J96" s="39"/>
+    </row>
+    <row r="97" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C97" s="39"/>
+      <c r="J97" s="39"/>
+    </row>
+    <row r="98" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C98" s="39"/>
+      <c r="J98" s="39"/>
+    </row>
+    <row r="99" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C99" s="39"/>
+      <c r="J99" s="39"/>
+    </row>
+    <row r="100" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="J100" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -2603,17 +3447,17 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:W80"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G5" sqref="G5"/>
+      <selection pane="bottomLeft" activeCell="H90" sqref="H90"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B1" s="12" t="s">
         <v>33</v>
       </c>
@@ -2621,7 +3465,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>32</v>
       </c>
@@ -2648,7 +3492,7 @@
       <c r="R2" s="14"/>
       <c r="S2" s="15"/>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="16"/>
       <c r="B3" s="17"/>
       <c r="C3" s="17"/>
@@ -2671,7 +3515,7 @@
       <c r="R3" s="17"/>
       <c r="S3" s="18"/>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="16"/>
       <c r="B4" s="17"/>
       <c r="C4" s="17"/>
@@ -2694,7 +3538,7 @@
       <c r="R4" s="17"/>
       <c r="S4" s="18"/>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="16"/>
       <c r="B5" s="17"/>
       <c r="C5" s="17"/>
@@ -2717,7 +3561,7 @@
       <c r="R5" s="17"/>
       <c r="S5" s="18"/>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="16"/>
       <c r="B6" s="17"/>
       <c r="C6" s="17"/>
@@ -2740,7 +3584,7 @@
       <c r="R6" s="17"/>
       <c r="S6" s="18"/>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="16"/>
       <c r="B7" s="17"/>
       <c r="C7" s="17"/>
@@ -2763,7 +3607,7 @@
       <c r="R7" s="17"/>
       <c r="S7" s="18"/>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="16"/>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -2786,7 +3630,7 @@
       <c r="R8" s="17"/>
       <c r="S8" s="18"/>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="16"/>
       <c r="B9" s="17"/>
       <c r="C9" s="17"/>
@@ -2809,7 +3653,7 @@
       <c r="R9" s="17"/>
       <c r="S9" s="18"/>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="16"/>
       <c r="B10" s="17"/>
       <c r="C10" s="17"/>
@@ -2832,7 +3676,7 @@
       <c r="R10" s="17"/>
       <c r="S10" s="18"/>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="16"/>
       <c r="B11" s="17"/>
       <c r="C11" s="17"/>
@@ -2853,7 +3697,7 @@
       <c r="R11" s="17"/>
       <c r="S11" s="18"/>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="16"/>
       <c r="B12" s="17" t="s">
         <v>55</v>
@@ -2878,7 +3722,7 @@
       <c r="R12" s="17"/>
       <c r="S12" s="18"/>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="16"/>
       <c r="B13" s="17"/>
       <c r="C13" s="17"/>
@@ -2901,7 +3745,7 @@
       <c r="R13" s="17"/>
       <c r="S13" s="18"/>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="16"/>
       <c r="B14" s="17"/>
       <c r="C14" s="17"/>
@@ -2924,7 +3768,7 @@
       <c r="R14" s="17"/>
       <c r="S14" s="18"/>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="16"/>
       <c r="B15" s="17"/>
       <c r="C15" s="17"/>
@@ -2947,7 +3791,7 @@
       <c r="R15" s="17"/>
       <c r="S15" s="18"/>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="16"/>
       <c r="B16" s="17"/>
       <c r="C16" s="17"/>
@@ -2970,7 +3814,7 @@
       <c r="R16" s="17"/>
       <c r="S16" s="18"/>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" s="16"/>
       <c r="B17" s="17"/>
       <c r="C17" s="17"/>
@@ -2993,7 +3837,7 @@
       <c r="R17" s="17"/>
       <c r="S17" s="18"/>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="16"/>
       <c r="B18" s="17"/>
       <c r="C18" s="17"/>
@@ -3016,7 +3860,7 @@
       <c r="R18" s="17"/>
       <c r="S18" s="18"/>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="16"/>
       <c r="B19" s="17"/>
       <c r="C19" s="17"/>
@@ -3039,7 +3883,7 @@
       <c r="R19" s="17"/>
       <c r="S19" s="18"/>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" s="16"/>
       <c r="B20" s="17"/>
       <c r="C20" s="17"/>
@@ -3062,7 +3906,7 @@
       <c r="R20" s="17"/>
       <c r="S20" s="18"/>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" s="16"/>
       <c r="B21" s="17"/>
       <c r="C21" s="17"/>
@@ -3085,7 +3929,7 @@
       <c r="R21" s="17"/>
       <c r="S21" s="18"/>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" s="16"/>
       <c r="B22" s="17"/>
       <c r="C22" s="17"/>
@@ -3108,7 +3952,7 @@
       <c r="R22" s="17"/>
       <c r="S22" s="18"/>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23" s="16"/>
       <c r="B23" s="17"/>
       <c r="C23" s="17"/>
@@ -3131,7 +3975,7 @@
       <c r="R23" s="17"/>
       <c r="S23" s="18"/>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" s="16"/>
       <c r="B24" s="17"/>
       <c r="C24" s="17"/>
@@ -3152,7 +3996,7 @@
       <c r="R24" s="17"/>
       <c r="S24" s="18"/>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" s="16"/>
       <c r="B25" s="17"/>
       <c r="C25" s="17"/>
@@ -3173,7 +4017,7 @@
       <c r="R25" s="17"/>
       <c r="S25" s="18"/>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26" s="16"/>
       <c r="B26" s="17"/>
       <c r="C26" s="17"/>
@@ -3194,7 +4038,7 @@
       <c r="R26" s="17"/>
       <c r="S26" s="18"/>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27" s="16"/>
       <c r="B27" s="17"/>
       <c r="C27" s="17"/>
@@ -3215,7 +4059,7 @@
       <c r="R27" s="17"/>
       <c r="S27" s="18"/>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28" s="16"/>
       <c r="B28" s="17"/>
       <c r="C28" s="17"/>
@@ -3236,7 +4080,7 @@
       <c r="R28" s="17"/>
       <c r="S28" s="18"/>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29" s="16"/>
       <c r="B29" s="17"/>
       <c r="C29" s="17"/>
@@ -3257,13 +4101,13 @@
       <c r="R29" s="17"/>
       <c r="S29" s="18"/>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30" s="16"/>
-      <c r="B30" s="35" t="s">
+      <c r="B30" s="41" t="s">
         <v>68</v>
       </c>
-      <c r="C30" s="35"/>
-      <c r="D30" s="35"/>
+      <c r="C30" s="41"/>
+      <c r="D30" s="41"/>
       <c r="E30" s="17"/>
       <c r="F30" s="17"/>
       <c r="G30" s="17"/>
@@ -3280,7 +4124,7 @@
       <c r="R30" s="17"/>
       <c r="S30" s="18"/>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A31" s="16"/>
       <c r="B31" s="17"/>
       <c r="C31" s="17"/>
@@ -3301,7 +4145,7 @@
       <c r="R31" s="17"/>
       <c r="S31" s="18"/>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A32" s="16"/>
       <c r="B32" s="17"/>
       <c r="C32" s="17"/>
@@ -3324,7 +4168,7 @@
       <c r="R32" s="17"/>
       <c r="S32" s="18"/>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A33" s="16"/>
       <c r="B33" s="17"/>
       <c r="C33" s="17"/>
@@ -3347,7 +4191,7 @@
       <c r="R33" s="17"/>
       <c r="S33" s="18"/>
     </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A34" s="16"/>
       <c r="B34" s="17"/>
       <c r="C34" s="17"/>
@@ -3368,7 +4212,7 @@
       <c r="R34" s="17"/>
       <c r="S34" s="18"/>
     </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A35" s="16"/>
       <c r="B35" s="17" t="s">
         <v>55</v>
@@ -3393,7 +4237,7 @@
       <c r="R35" s="17"/>
       <c r="S35" s="18"/>
     </row>
-    <row r="36" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A36" s="16"/>
       <c r="B36" s="17"/>
       <c r="C36" s="17"/>
@@ -3416,7 +4260,7 @@
       <c r="R36" s="17"/>
       <c r="S36" s="18"/>
     </row>
-    <row r="37" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A37" s="16"/>
       <c r="B37" s="17"/>
       <c r="C37" s="17"/>
@@ -3439,7 +4283,7 @@
       <c r="R37" s="17"/>
       <c r="S37" s="18"/>
     </row>
-    <row r="38" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A38" s="16"/>
       <c r="B38" s="17"/>
       <c r="C38" s="17"/>
@@ -3462,7 +4306,7 @@
       <c r="R38" s="17"/>
       <c r="S38" s="18"/>
     </row>
-    <row r="39" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A39" s="16"/>
       <c r="B39" s="17"/>
       <c r="C39" s="17"/>
@@ -3474,18 +4318,18 @@
       <c r="G39" s="17"/>
       <c r="H39" s="17"/>
       <c r="I39" s="17"/>
-      <c r="J39" s="36"/>
-      <c r="K39" s="36"/>
-      <c r="L39" s="36"/>
-      <c r="M39" s="36"/>
-      <c r="N39" s="36"/>
-      <c r="O39" s="36"/>
+      <c r="J39" s="26"/>
+      <c r="K39" s="26"/>
+      <c r="L39" s="26"/>
+      <c r="M39" s="26"/>
+      <c r="N39" s="26"/>
+      <c r="O39" s="26"/>
       <c r="P39" s="17"/>
       <c r="Q39" s="17"/>
       <c r="R39" s="17"/>
       <c r="S39" s="18"/>
     </row>
-    <row r="40" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A40" s="16"/>
       <c r="B40" s="17" t="s">
         <v>72</v>
@@ -3510,11 +4354,11 @@
       <c r="R40" s="17"/>
       <c r="S40" s="18"/>
     </row>
-    <row r="41" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A41" s="16"/>
       <c r="B41" s="17"/>
       <c r="C41" s="17"/>
-      <c r="D41" s="37" t="s">
+      <c r="D41" s="27" t="s">
         <v>71</v>
       </c>
       <c r="E41" s="17"/>
@@ -3533,7 +4377,7 @@
       <c r="R41" s="17"/>
       <c r="S41" s="18"/>
     </row>
-    <row r="42" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A42" s="19"/>
       <c r="B42" s="20"/>
       <c r="C42" s="20"/>
@@ -3554,7 +4398,7 @@
       <c r="R42" s="20"/>
       <c r="S42" s="21"/>
     </row>
-    <row r="44" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A44" s="13" t="s">
         <v>76</v>
       </c>
@@ -3581,12 +4425,12 @@
       <c r="V44" s="14"/>
       <c r="W44" s="15"/>
     </row>
-    <row r="45" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A45" s="38"/>
-      <c r="B45" s="39" t="s">
+    <row r="45" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="28"/>
+      <c r="B45" s="42" t="s">
         <v>101</v>
       </c>
-      <c r="C45" s="39"/>
+      <c r="C45" s="42"/>
       <c r="D45" s="17"/>
       <c r="E45" s="17"/>
       <c r="F45" s="17"/>
@@ -3608,7 +4452,7 @@
       <c r="V45" s="17"/>
       <c r="W45" s="18"/>
     </row>
-    <row r="46" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A46" s="16"/>
       <c r="B46" s="17"/>
       <c r="C46" s="17"/>
@@ -3635,7 +4479,7 @@
       <c r="V46" s="17"/>
       <c r="W46" s="18"/>
     </row>
-    <row r="47" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A47" s="16"/>
       <c r="B47" s="17"/>
       <c r="C47" s="17"/>
@@ -3662,7 +4506,7 @@
       <c r="V47" s="17"/>
       <c r="W47" s="18"/>
     </row>
-    <row r="48" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A48" s="16"/>
       <c r="B48" s="17"/>
       <c r="C48" s="17"/>
@@ -3689,7 +4533,7 @@
       <c r="V48" s="17"/>
       <c r="W48" s="18"/>
     </row>
-    <row r="49" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A49" s="16"/>
       <c r="B49" s="17"/>
       <c r="C49" s="17"/>
@@ -3716,7 +4560,7 @@
       <c r="V49" s="17"/>
       <c r="W49" s="18"/>
     </row>
-    <row r="50" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A50" s="16"/>
       <c r="B50" s="17"/>
       <c r="C50" s="17"/>
@@ -3743,7 +4587,7 @@
       <c r="V50" s="17"/>
       <c r="W50" s="18"/>
     </row>
-    <row r="51" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A51" s="16"/>
       <c r="B51" s="17"/>
       <c r="C51" s="17"/>
@@ -3770,7 +4614,7 @@
       <c r="V51" s="17"/>
       <c r="W51" s="18"/>
     </row>
-    <row r="52" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A52" s="16"/>
       <c r="B52" s="17"/>
       <c r="C52" s="17"/>
@@ -3797,7 +4641,7 @@
       <c r="V52" s="17"/>
       <c r="W52" s="18"/>
     </row>
-    <row r="53" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A53" s="16"/>
       <c r="B53" s="17"/>
       <c r="C53" s="17"/>
@@ -3824,7 +4668,7 @@
       <c r="V53" s="17"/>
       <c r="W53" s="18"/>
     </row>
-    <row r="54" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A54" s="16"/>
       <c r="B54" s="17"/>
       <c r="C54" s="17"/>
@@ -3851,20 +4695,20 @@
       <c r="V54" s="17"/>
       <c r="W54" s="18"/>
     </row>
-    <row r="55" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A55" s="16"/>
       <c r="B55" s="17"/>
       <c r="C55" s="17"/>
       <c r="D55" s="17"/>
       <c r="E55" s="17"/>
       <c r="F55" s="17"/>
-      <c r="G55" s="40" t="s">
+      <c r="G55" s="29" t="s">
         <v>85</v>
       </c>
-      <c r="H55" s="40"/>
-      <c r="I55" s="40"/>
-      <c r="J55" s="40"/>
-      <c r="K55" s="40"/>
+      <c r="H55" s="29"/>
+      <c r="I55" s="29"/>
+      <c r="J55" s="29"/>
+      <c r="K55" s="29"/>
       <c r="L55" s="17"/>
       <c r="M55" s="17"/>
       <c r="N55" s="17"/>
@@ -3878,7 +4722,7 @@
       <c r="V55" s="17"/>
       <c r="W55" s="18"/>
     </row>
-    <row r="56" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A56" s="16"/>
       <c r="B56" s="17"/>
       <c r="C56" s="17"/>
@@ -3905,7 +4749,7 @@
       <c r="V56" s="17"/>
       <c r="W56" s="18"/>
     </row>
-    <row r="57" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A57" s="16"/>
       <c r="B57" s="17"/>
       <c r="C57" s="17"/>
@@ -3914,15 +4758,15 @@
       <c r="F57" s="17"/>
       <c r="G57" s="17"/>
       <c r="H57" s="17"/>
-      <c r="I57" s="36" t="s">
+      <c r="I57" s="26" t="s">
         <v>87</v>
       </c>
-      <c r="J57" s="36"/>
-      <c r="K57" s="36"/>
-      <c r="L57" s="36"/>
-      <c r="M57" s="36"/>
-      <c r="N57" s="36"/>
-      <c r="O57" s="36"/>
+      <c r="J57" s="26"/>
+      <c r="K57" s="26"/>
+      <c r="L57" s="26"/>
+      <c r="M57" s="26"/>
+      <c r="N57" s="26"/>
+      <c r="O57" s="26"/>
       <c r="P57" s="17"/>
       <c r="Q57" s="17"/>
       <c r="R57" s="17"/>
@@ -3932,7 +4776,7 @@
       <c r="V57" s="17"/>
       <c r="W57" s="18"/>
     </row>
-    <row r="58" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A58" s="16"/>
       <c r="B58" s="17"/>
       <c r="C58" s="17"/>
@@ -3959,7 +4803,7 @@
       <c r="V58" s="17"/>
       <c r="W58" s="18"/>
     </row>
-    <row r="59" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A59" s="16"/>
       <c r="B59" s="17"/>
       <c r="C59" s="17"/>
@@ -3986,7 +4830,7 @@
       <c r="V59" s="17"/>
       <c r="W59" s="18"/>
     </row>
-    <row r="60" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A60" s="16"/>
       <c r="B60" s="17"/>
       <c r="C60" s="17"/>
@@ -3998,22 +4842,22 @@
       <c r="I60" s="17"/>
       <c r="J60" s="17"/>
       <c r="K60" s="17"/>
-      <c r="L60" s="41" t="s">
+      <c r="L60" s="30" t="s">
         <v>89</v>
       </c>
-      <c r="M60" s="41"/>
-      <c r="N60" s="41"/>
-      <c r="O60" s="41"/>
-      <c r="P60" s="41"/>
-      <c r="Q60" s="41"/>
-      <c r="R60" s="41"/>
-      <c r="S60" s="41"/>
-      <c r="T60" s="41"/>
-      <c r="U60" s="41"/>
+      <c r="M60" s="30"/>
+      <c r="N60" s="30"/>
+      <c r="O60" s="30"/>
+      <c r="P60" s="30"/>
+      <c r="Q60" s="30"/>
+      <c r="R60" s="30"/>
+      <c r="S60" s="30"/>
+      <c r="T60" s="30"/>
+      <c r="U60" s="30"/>
       <c r="V60" s="17"/>
       <c r="W60" s="18"/>
     </row>
-    <row r="61" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A61" s="16"/>
       <c r="B61" s="17"/>
       <c r="C61" s="17"/>
@@ -4025,22 +4869,22 @@
       <c r="I61" s="17"/>
       <c r="J61" s="17"/>
       <c r="K61" s="17"/>
-      <c r="L61" s="41"/>
-      <c r="M61" s="41" t="s">
+      <c r="L61" s="30"/>
+      <c r="M61" s="30" t="s">
         <v>90</v>
       </c>
-      <c r="N61" s="41"/>
-      <c r="O61" s="41"/>
-      <c r="P61" s="41"/>
-      <c r="Q61" s="41"/>
-      <c r="R61" s="41"/>
-      <c r="S61" s="41"/>
-      <c r="T61" s="41"/>
-      <c r="U61" s="41"/>
+      <c r="N61" s="30"/>
+      <c r="O61" s="30"/>
+      <c r="P61" s="30"/>
+      <c r="Q61" s="30"/>
+      <c r="R61" s="30"/>
+      <c r="S61" s="30"/>
+      <c r="T61" s="30"/>
+      <c r="U61" s="30"/>
       <c r="V61" s="17"/>
       <c r="W61" s="18"/>
     </row>
-    <row r="62" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A62" s="16"/>
       <c r="B62" s="17"/>
       <c r="C62" s="17"/>
@@ -4052,22 +4896,22 @@
       <c r="I62" s="17"/>
       <c r="J62" s="17"/>
       <c r="K62" s="17"/>
-      <c r="L62" s="41"/>
-      <c r="M62" s="41" t="s">
+      <c r="L62" s="30"/>
+      <c r="M62" s="30" t="s">
         <v>91</v>
       </c>
-      <c r="N62" s="41"/>
-      <c r="O62" s="41"/>
-      <c r="P62" s="41"/>
-      <c r="Q62" s="41"/>
-      <c r="R62" s="41"/>
-      <c r="S62" s="41"/>
-      <c r="T62" s="41"/>
-      <c r="U62" s="41"/>
+      <c r="N62" s="30"/>
+      <c r="O62" s="30"/>
+      <c r="P62" s="30"/>
+      <c r="Q62" s="30"/>
+      <c r="R62" s="30"/>
+      <c r="S62" s="30"/>
+      <c r="T62" s="30"/>
+      <c r="U62" s="30"/>
       <c r="V62" s="17"/>
       <c r="W62" s="18"/>
     </row>
-    <row r="63" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A63" s="16"/>
       <c r="B63" s="17"/>
       <c r="C63" s="17"/>
@@ -4079,22 +4923,22 @@
       <c r="I63" s="17"/>
       <c r="J63" s="17"/>
       <c r="K63" s="17"/>
-      <c r="L63" s="41" t="s">
+      <c r="L63" s="30" t="s">
         <v>92</v>
       </c>
-      <c r="M63" s="41"/>
-      <c r="N63" s="41"/>
-      <c r="O63" s="41"/>
-      <c r="P63" s="41"/>
-      <c r="Q63" s="41"/>
-      <c r="R63" s="41"/>
-      <c r="S63" s="41"/>
-      <c r="T63" s="41"/>
-      <c r="U63" s="41"/>
+      <c r="M63" s="30"/>
+      <c r="N63" s="30"/>
+      <c r="O63" s="30"/>
+      <c r="P63" s="30"/>
+      <c r="Q63" s="30"/>
+      <c r="R63" s="30"/>
+      <c r="S63" s="30"/>
+      <c r="T63" s="30"/>
+      <c r="U63" s="30"/>
       <c r="V63" s="17"/>
       <c r="W63" s="18"/>
     </row>
-    <row r="64" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A64" s="16"/>
       <c r="B64" s="17"/>
       <c r="C64" s="17"/>
@@ -4121,7 +4965,7 @@
       <c r="V64" s="17"/>
       <c r="W64" s="18"/>
     </row>
-    <row r="65" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A65" s="16"/>
       <c r="B65" s="17"/>
       <c r="C65" s="17"/>
@@ -4148,7 +4992,7 @@
       <c r="V65" s="17"/>
       <c r="W65" s="18"/>
     </row>
-    <row r="66" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A66" s="16"/>
       <c r="B66" s="17"/>
       <c r="C66" s="17"/>
@@ -4175,7 +5019,7 @@
       <c r="V66" s="17"/>
       <c r="W66" s="18"/>
     </row>
-    <row r="67" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A67" s="16"/>
       <c r="B67" s="17"/>
       <c r="C67" s="17"/>
@@ -4186,23 +5030,23 @@
       <c r="H67" s="17"/>
       <c r="I67" s="17"/>
       <c r="J67" s="17"/>
-      <c r="K67" s="42" t="s">
+      <c r="K67" s="31" t="s">
         <v>96</v>
       </c>
-      <c r="L67" s="42"/>
-      <c r="M67" s="42"/>
-      <c r="N67" s="42"/>
-      <c r="O67" s="42"/>
-      <c r="P67" s="42"/>
-      <c r="Q67" s="42"/>
-      <c r="R67" s="42"/>
-      <c r="S67" s="42"/>
+      <c r="L67" s="31"/>
+      <c r="M67" s="31"/>
+      <c r="N67" s="31"/>
+      <c r="O67" s="31"/>
+      <c r="P67" s="31"/>
+      <c r="Q67" s="31"/>
+      <c r="R67" s="31"/>
+      <c r="S67" s="31"/>
       <c r="T67" s="17"/>
       <c r="U67" s="17"/>
       <c r="V67" s="17"/>
       <c r="W67" s="18"/>
     </row>
-    <row r="68" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A68" s="16"/>
       <c r="B68" s="17"/>
       <c r="C68" s="17"/>
@@ -4229,7 +5073,7 @@
       <c r="V68" s="17"/>
       <c r="W68" s="18"/>
     </row>
-    <row r="69" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A69" s="16"/>
       <c r="B69" s="17"/>
       <c r="C69" s="17"/>
@@ -4256,7 +5100,7 @@
       <c r="V69" s="17"/>
       <c r="W69" s="18"/>
     </row>
-    <row r="70" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A70" s="16"/>
       <c r="B70" s="17"/>
       <c r="C70" s="17"/>
@@ -4283,7 +5127,7 @@
       <c r="V70" s="17"/>
       <c r="W70" s="18"/>
     </row>
-    <row r="71" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="71" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A71" s="16"/>
       <c r="B71" s="17"/>
       <c r="C71" s="17"/>
@@ -4310,7 +5154,7 @@
       <c r="V71" s="17"/>
       <c r="W71" s="18"/>
     </row>
-    <row r="72" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A72" s="16"/>
       <c r="B72" s="17"/>
       <c r="C72" s="17"/>
@@ -4337,7 +5181,7 @@
       <c r="V72" s="17"/>
       <c r="W72" s="18"/>
     </row>
-    <row r="73" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A73" s="16"/>
       <c r="B73" s="17"/>
       <c r="C73" s="17"/>
@@ -4364,7 +5208,7 @@
       <c r="V73" s="17"/>
       <c r="W73" s="18"/>
     </row>
-    <row r="74" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="74" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A74" s="16"/>
       <c r="B74" s="17"/>
       <c r="C74" s="17"/>
@@ -4391,7 +5235,7 @@
       <c r="V74" s="17"/>
       <c r="W74" s="18"/>
     </row>
-    <row r="75" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="75" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A75" s="16"/>
       <c r="B75" s="17"/>
       <c r="C75" s="17"/>
@@ -4418,7 +5262,7 @@
       <c r="V75" s="17"/>
       <c r="W75" s="18"/>
     </row>
-    <row r="76" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="76" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A76" s="16"/>
       <c r="B76" s="17"/>
       <c r="C76" s="17"/>
@@ -4445,7 +5289,7 @@
       <c r="V76" s="17"/>
       <c r="W76" s="18"/>
     </row>
-    <row r="77" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="77" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A77" s="16"/>
       <c r="B77" s="17"/>
       <c r="C77" s="17"/>
@@ -4472,7 +5316,7 @@
       <c r="V77" s="17"/>
       <c r="W77" s="18"/>
     </row>
-    <row r="78" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="78" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A78" s="16"/>
       <c r="B78" s="17"/>
       <c r="C78" s="17"/>
@@ -4497,13 +5341,13 @@
       <c r="V78" s="17"/>
       <c r="W78" s="18"/>
     </row>
-    <row r="79" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="79" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A79" s="16"/>
-      <c r="B79" s="35" t="s">
+      <c r="B79" s="41" t="s">
         <v>68</v>
       </c>
-      <c r="C79" s="35"/>
-      <c r="D79" s="35"/>
+      <c r="C79" s="41"/>
+      <c r="D79" s="41"/>
       <c r="E79" s="17"/>
       <c r="F79" s="17"/>
       <c r="G79" s="17"/>
@@ -4524,7 +5368,7 @@
       <c r="V79" s="17"/>
       <c r="W79" s="18"/>
     </row>
-    <row r="80" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="80" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A80" s="19"/>
       <c r="B80" s="20"/>
       <c r="C80" s="20"/>
@@ -4562,4 +5406,598 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1265DB25-31DB-49BB-815F-99DD6BADE696}">
+  <dimension ref="A1:F30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="16384" width="8.88671875" style="43"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="16.2" x14ac:dyDescent="0.4">
+      <c r="A1" s="44" t="s">
+        <v>167</v>
+      </c>
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="51" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" s="43" t="s">
+        <v>147</v>
+      </c>
+      <c r="B2" s="43" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" s="43" t="s">
+        <v>149</v>
+      </c>
+      <c r="B3" s="43" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B4" s="43" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D5" s="50" t="s">
+        <v>151</v>
+      </c>
+      <c r="E5" s="50"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D6" s="53" t="s">
+        <v>152</v>
+      </c>
+      <c r="E6" s="50"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D7" s="43" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D8" s="43" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D9" s="43" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D10" s="43" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D11" s="43" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D13" s="43" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D14" s="43" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D15" s="43" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D16" s="43" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="D17" s="50" t="s">
+        <v>161</v>
+      </c>
+      <c r="E17" s="50"/>
+      <c r="F17" s="50"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="D18" s="52" t="s">
+        <v>162</v>
+      </c>
+      <c r="E18" s="50"/>
+      <c r="F18" s="50"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="D19" s="52" t="s">
+        <v>168</v>
+      </c>
+      <c r="E19" s="50"/>
+      <c r="F19" s="50"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="D20" s="52" t="s">
+        <v>163</v>
+      </c>
+      <c r="E20" s="50"/>
+      <c r="F20" s="50"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C21" s="43" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="16.2" x14ac:dyDescent="0.4">
+      <c r="A22" s="43" t="s">
+        <v>184</v>
+      </c>
+      <c r="B22" s="43" t="s">
+        <v>187</v>
+      </c>
+      <c r="D22" s="75"/>
+      <c r="E22" s="75"/>
+      <c r="F22" s="75"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E23" s="43" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F24" s="43" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F25" s="43" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F26" s="43" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E27" s="43" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="D28" s="43" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A29" s="43" t="s">
+        <v>192</v>
+      </c>
+      <c r="B29" s="43" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A30" s="43" t="s">
+        <v>194</v>
+      </c>
+      <c r="B30" s="43" t="s">
+        <v>193</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="D1" location="共通方法!A1" display="共同方法" xr:uid="{6A01D1A9-E8CA-473C-B6A2-AAF668B2C7A8}"/>
+    <hyperlink ref="D6" location="共通方法!D2" display="enableTooltip();" xr:uid="{7E16EDA0-8F2C-4909-970D-75353C94139A}"/>
+    <hyperlink ref="D18" location="共通方法!D3" display="setSearchEnabled();" xr:uid="{C0D77DE3-81EC-43A6-8651-BE93550F4121}"/>
+    <hyperlink ref="D19" location="共通方法!D5" display="setUpdateDisabled();" xr:uid="{A0752034-372F-4799-98A0-1C27D15B1968}"/>
+    <hyperlink ref="D20" location="共通方法!D7" display="setRegisteredEnabled();" xr:uid="{7E6FFF63-AAE5-4AF2-93EA-E3A5BD5DC973}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C70B497F-AB8C-4CC4-8928-CCD1AC2AD8DB}">
+  <dimension ref="B1:K22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="E18" sqref="E18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="1.88671875" style="43" customWidth="1"/>
+    <col min="2" max="2" width="33.6640625" style="45" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.88671875" style="43"/>
+    <col min="4" max="4" width="24.33203125" style="43" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.6640625" style="45" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.77734375" style="43" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="31.33203125" style="45" customWidth="1"/>
+    <col min="8" max="8" width="23.77734375" style="43" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.88671875" style="43"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:11" ht="16.8" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B1" s="49" t="s">
+        <v>104</v>
+      </c>
+      <c r="C1" s="47" t="s">
+        <v>105</v>
+      </c>
+      <c r="D1" s="47" t="s">
+        <v>106</v>
+      </c>
+      <c r="E1" s="48" t="s">
+        <v>107</v>
+      </c>
+      <c r="F1" s="46" t="s">
+        <v>124</v>
+      </c>
+      <c r="G1" s="49" t="s">
+        <v>134</v>
+      </c>
+      <c r="H1" s="46" t="s">
+        <v>129</v>
+      </c>
+      <c r="I1" s="54" t="s">
+        <v>183</v>
+      </c>
+      <c r="J1" s="54"/>
+      <c r="K1" s="54"/>
+    </row>
+    <row r="2" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B2" s="55" t="s">
+        <v>103</v>
+      </c>
+      <c r="C2" s="56" t="s">
+        <v>108</v>
+      </c>
+      <c r="D2" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="E2" s="58" t="s">
+        <v>110</v>
+      </c>
+      <c r="F2" s="57"/>
+      <c r="G2" s="58"/>
+      <c r="H2" s="59"/>
+    </row>
+    <row r="3" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B3" s="60"/>
+      <c r="C3" s="61"/>
+      <c r="D3" s="62" t="s">
+        <v>111</v>
+      </c>
+      <c r="E3" s="63" t="s">
+        <v>113</v>
+      </c>
+      <c r="F3" s="62"/>
+      <c r="G3" s="63"/>
+      <c r="H3" s="64"/>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B4" s="60"/>
+      <c r="C4" s="61"/>
+      <c r="D4" s="62" t="s">
+        <v>112</v>
+      </c>
+      <c r="E4" s="63" t="s">
+        <v>114</v>
+      </c>
+      <c r="F4" s="62" t="s">
+        <v>185</v>
+      </c>
+      <c r="G4" s="63" t="s">
+        <v>186</v>
+      </c>
+      <c r="H4" s="64"/>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B5" s="60"/>
+      <c r="C5" s="61"/>
+      <c r="D5" s="62" t="s">
+        <v>115</v>
+      </c>
+      <c r="E5" s="63" t="s">
+        <v>116</v>
+      </c>
+      <c r="F5" s="62"/>
+      <c r="G5" s="63"/>
+      <c r="H5" s="64"/>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B6" s="60"/>
+      <c r="C6" s="61"/>
+      <c r="D6" s="62" t="s">
+        <v>117</v>
+      </c>
+      <c r="E6" s="63" t="s">
+        <v>121</v>
+      </c>
+      <c r="F6" s="62" t="s">
+        <v>185</v>
+      </c>
+      <c r="G6" s="63" t="s">
+        <v>186</v>
+      </c>
+      <c r="H6" s="64"/>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B7" s="60"/>
+      <c r="C7" s="61"/>
+      <c r="D7" s="62" t="s">
+        <v>118</v>
+      </c>
+      <c r="E7" s="63" t="s">
+        <v>120</v>
+      </c>
+      <c r="F7" s="62"/>
+      <c r="G7" s="63"/>
+      <c r="H7" s="64"/>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B8" s="60"/>
+      <c r="C8" s="61"/>
+      <c r="D8" s="62" t="s">
+        <v>119</v>
+      </c>
+      <c r="E8" s="63" t="s">
+        <v>114</v>
+      </c>
+      <c r="F8" s="62" t="s">
+        <v>185</v>
+      </c>
+      <c r="G8" s="63" t="s">
+        <v>186</v>
+      </c>
+      <c r="H8" s="64"/>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B9" s="60"/>
+      <c r="C9" s="61"/>
+      <c r="D9" s="65" t="s">
+        <v>122</v>
+      </c>
+      <c r="E9" s="66" t="s">
+        <v>123</v>
+      </c>
+      <c r="F9" s="62" t="s">
+        <v>125</v>
+      </c>
+      <c r="G9" s="63"/>
+      <c r="H9" s="64"/>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B10" s="60"/>
+      <c r="C10" s="61"/>
+      <c r="D10" s="65"/>
+      <c r="E10" s="66"/>
+      <c r="F10" s="62" t="s">
+        <v>126</v>
+      </c>
+      <c r="G10" s="63"/>
+      <c r="H10" s="64"/>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B11" s="60"/>
+      <c r="C11" s="61"/>
+      <c r="D11" s="65"/>
+      <c r="E11" s="66"/>
+      <c r="F11" s="62" t="s">
+        <v>127</v>
+      </c>
+      <c r="G11" s="63"/>
+      <c r="H11" s="64"/>
+    </row>
+    <row r="12" spans="2:11" ht="31.2" x14ac:dyDescent="0.35">
+      <c r="B12" s="60"/>
+      <c r="C12" s="61"/>
+      <c r="D12" s="62" t="s">
+        <v>128</v>
+      </c>
+      <c r="E12" s="63" t="s">
+        <v>173</v>
+      </c>
+      <c r="F12" s="62"/>
+      <c r="G12" s="63"/>
+      <c r="H12" s="64"/>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B13" s="60"/>
+      <c r="C13" s="61"/>
+      <c r="D13" s="65" t="s">
+        <v>130</v>
+      </c>
+      <c r="E13" s="63" t="s">
+        <v>131</v>
+      </c>
+      <c r="F13" s="62" t="s">
+        <v>132</v>
+      </c>
+      <c r="G13" s="63" t="s">
+        <v>135</v>
+      </c>
+      <c r="H13" s="64"/>
+    </row>
+    <row r="14" spans="2:11" ht="78" x14ac:dyDescent="0.35">
+      <c r="B14" s="60"/>
+      <c r="C14" s="61"/>
+      <c r="D14" s="65"/>
+      <c r="E14" s="63" t="s">
+        <v>131</v>
+      </c>
+      <c r="F14" s="62" t="s">
+        <v>133</v>
+      </c>
+      <c r="G14" s="63" t="s">
+        <v>136</v>
+      </c>
+      <c r="H14" s="64"/>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B15" s="60"/>
+      <c r="C15" s="61"/>
+      <c r="D15" s="62" t="s">
+        <v>137</v>
+      </c>
+      <c r="E15" s="63" t="s">
+        <v>138</v>
+      </c>
+      <c r="F15" s="62"/>
+      <c r="G15" s="63"/>
+      <c r="H15" s="64"/>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B16" s="60"/>
+      <c r="C16" s="61"/>
+      <c r="D16" s="65" t="s">
+        <v>139</v>
+      </c>
+      <c r="E16" s="66" t="s">
+        <v>140</v>
+      </c>
+      <c r="F16" s="62" t="s">
+        <v>141</v>
+      </c>
+      <c r="G16" s="63"/>
+      <c r="H16" s="64"/>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B17" s="60"/>
+      <c r="C17" s="61"/>
+      <c r="D17" s="65"/>
+      <c r="E17" s="66"/>
+      <c r="F17" s="62" t="s">
+        <v>142</v>
+      </c>
+      <c r="G17" s="63"/>
+      <c r="H17" s="64"/>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B18" s="60"/>
+      <c r="C18" s="61"/>
+      <c r="D18" s="62" t="s">
+        <v>143</v>
+      </c>
+      <c r="E18" s="63" t="s">
+        <v>144</v>
+      </c>
+      <c r="F18" s="62" t="s">
+        <v>145</v>
+      </c>
+      <c r="G18" s="63" t="s">
+        <v>146</v>
+      </c>
+      <c r="H18" s="64"/>
+    </row>
+    <row r="19" spans="2:8" ht="31.2" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B19" s="60" t="s">
+        <v>169</v>
+      </c>
+      <c r="C19" s="65" t="s">
+        <v>43</v>
+      </c>
+      <c r="D19" s="67" t="s">
+        <v>170</v>
+      </c>
+      <c r="E19" s="68" t="s">
+        <v>174</v>
+      </c>
+      <c r="F19" s="62" t="s">
+        <v>171</v>
+      </c>
+      <c r="G19" s="63" t="s">
+        <v>175</v>
+      </c>
+      <c r="H19" s="69" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" ht="46.2" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B20" s="60"/>
+      <c r="C20" s="65"/>
+      <c r="D20" s="67"/>
+      <c r="E20" s="68"/>
+      <c r="F20" s="62" t="s">
+        <v>172</v>
+      </c>
+      <c r="G20" s="63" t="s">
+        <v>176</v>
+      </c>
+      <c r="H20" s="69" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" ht="31.2" x14ac:dyDescent="0.35">
+      <c r="B21" s="70" t="s">
+        <v>178</v>
+      </c>
+      <c r="C21" s="62" t="s">
+        <v>177</v>
+      </c>
+      <c r="D21" s="62" t="s">
+        <v>179</v>
+      </c>
+      <c r="E21" s="63" t="s">
+        <v>180</v>
+      </c>
+      <c r="F21" s="62" t="s">
+        <v>181</v>
+      </c>
+      <c r="G21" s="63" t="s">
+        <v>182</v>
+      </c>
+      <c r="H21" s="64"/>
+    </row>
+    <row r="22" spans="2:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B22" s="71"/>
+      <c r="C22" s="72"/>
+      <c r="D22" s="72"/>
+      <c r="E22" s="73"/>
+      <c r="F22" s="72"/>
+      <c r="G22" s="73"/>
+      <c r="H22" s="74"/>
+    </row>
+  </sheetData>
+  <mergeCells count="11">
+    <mergeCell ref="B2:B18"/>
+    <mergeCell ref="C2:C18"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="D9:D11"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="E9:E11"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="H19" location="共通方法!D13" display="confirmTransitionHtml" xr:uid="{4D7D729B-1636-477F-94B0-3E05775C8EC2}"/>
+    <hyperlink ref="H20" location="共通方法!D21" display="setMenuContent" xr:uid="{E1827E0E-C13B-4737-9826-6131F70B5DC4}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>